<commit_message>
Editar listas de peliculas del usuario y product backlog actualizado
</commit_message>
<xml_diff>
--- a/ToDo/Product Backlog.xlsx
+++ b/ToDo/Product Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minie\Desktop\UMA\Tercer Curso\2do cuatrimestre\Tecnologías de Aplicaciones Web\Trabajo en grupo\ArkhamMovies\ToDo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF2A13A-77AF-4B8D-8D19-9815992E7E80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D0B3C7-80EB-460B-86F2-6AC30C2239DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{391AEB77-1329-4C84-A561-AE54ADC33E64}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="59">
   <si>
     <t>ID</t>
   </si>
@@ -571,9 +571,6 @@
   </si>
   <si>
     <t>Hecho</t>
-  </si>
-  <si>
-    <t>Pendiente la edición</t>
   </si>
   <si>
     <t>Pendiente orden personalizado</t>
@@ -724,7 +721,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -732,13 +729,19 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -748,6 +751,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -757,53 +769,35 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1141,8 +1135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D14C92F-3F4B-401B-9B84-B21C184BF8CD}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1174,506 +1168,492 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="11" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="4" t="s">
+      <c r="A3" s="9"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="13"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="12"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="4" t="s">
+      <c r="A4" s="9"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="13"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="12"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="4" t="s">
+      <c r="A5" s="10"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="14"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="13"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="25" t="s">
+      <c r="E6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="11" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="13"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="12"/>
     </row>
     <row r="8" spans="1:6" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="9" t="s">
+      <c r="A8" s="9"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="13"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="12"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="14"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="13"/>
     </row>
     <row r="10" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="25" t="s">
+      <c r="E10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="11" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="13"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="12"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="9" t="s">
+      <c r="A12" s="9"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="13"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="12"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="14"/>
+      <c r="A13" s="10"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="13"/>
     </row>
     <row r="14" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="25" t="s">
+      <c r="E14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="11" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="13"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="12"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="15" t="s">
+      <c r="A16" s="9"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="10"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="13"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="12"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="14"/>
+      <c r="A17" s="10"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="13"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E18" s="25" t="s">
+      <c r="E18" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F18" s="12" t="s">
+      <c r="F18" s="11" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="13"/>
+      <c r="A19" s="9"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="12"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="15" t="s">
+      <c r="A20" s="9"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="10"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="13"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="12"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="14"/>
+      <c r="A21" s="10"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="13"/>
     </row>
     <row r="22" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="D22" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E22" s="25" t="s">
+      <c r="E22" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F22" s="17" t="s">
-        <v>58</v>
+      <c r="F22" s="23" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="4" t="s">
+      <c r="A23" s="9"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D23" s="10"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="18"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="24"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24" s="10"/>
+      <c r="A24" s="9"/>
+      <c r="B24" s="15"/>
       <c r="C24" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D24" s="10"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="18"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="24"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="4" t="s">
+      <c r="A25" s="10"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D25" s="11"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="19"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="25"/>
     </row>
     <row r="26" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="D26" s="9" t="s">
+      <c r="D26" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="E26" s="25" t="s">
+      <c r="E26" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F26" s="12" t="s">
+      <c r="F26" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
-      <c r="B27" s="10"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="13"/>
+      <c r="A27" s="9"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="12"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="13"/>
+      <c r="A28" s="9"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="12"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="8"/>
-      <c r="B29" s="11"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="14"/>
+      <c r="A29" s="10"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="13"/>
     </row>
     <row r="30" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="B30" s="14" t="s">
         <v>15</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D30" s="9" t="s">
+      <c r="D30" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E30" s="20" t="s">
+      <c r="E30" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F30" s="12" t="s">
+      <c r="F30" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
-      <c r="B31" s="10"/>
+      <c r="A31" s="9"/>
+      <c r="B31" s="15"/>
       <c r="C31" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D31" s="10"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="13"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="12"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
-      <c r="B32" s="10"/>
+      <c r="A32" s="9"/>
+      <c r="B32" s="15"/>
       <c r="C32" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D32" s="10"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="13"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="12"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="8"/>
-      <c r="B33" s="11"/>
+      <c r="A33" s="10"/>
+      <c r="B33" s="16"/>
       <c r="C33" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D33" s="11"/>
-      <c r="E33" s="22"/>
-      <c r="F33" s="14"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="13"/>
     </row>
     <row r="34" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="B34" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C34" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D34" s="9" t="s">
+      <c r="D34" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E34" s="20" t="s">
+      <c r="E34" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F34" s="12" t="s">
+      <c r="F34" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="7"/>
-      <c r="B35" s="10"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="21"/>
-      <c r="F35" s="13"/>
+      <c r="A35" s="9"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="12"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="7"/>
-      <c r="B36" s="10"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="21"/>
-      <c r="F36" s="13"/>
+      <c r="A36" s="9"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="12"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="8"/>
-      <c r="B37" s="11"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="22"/>
-      <c r="F37" s="14"/>
+      <c r="A37" s="10"/>
+      <c r="B37" s="16"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="13"/>
     </row>
     <row r="38" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
+      <c r="A38" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B38" s="9" t="s">
+      <c r="B38" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="C38" s="15" t="s">
+      <c r="C38" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="D38" s="9" t="s">
+      <c r="D38" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E38" s="20" t="s">
+      <c r="E38" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F38" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="G38" s="5"/>
+      <c r="F38" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="G38" s="4"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="7"/>
-      <c r="B39" s="10"/>
-      <c r="C39" s="23"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="21"/>
-      <c r="F39" s="18"/>
+      <c r="A39" s="9"/>
+      <c r="B39" s="15"/>
+      <c r="C39" s="21"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="24"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="7"/>
-      <c r="B40" s="10"/>
-      <c r="C40" s="6" t="s">
+      <c r="A40" s="9"/>
+      <c r="B40" s="15"/>
+      <c r="C40" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D40" s="10"/>
-      <c r="E40" s="21"/>
-      <c r="F40" s="18"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="24"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="8"/>
-      <c r="B41" s="11"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="22"/>
-      <c r="F41" s="19"/>
+      <c r="A41" s="10"/>
+      <c r="B41" s="16"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="62">
-    <mergeCell ref="E2:E5"/>
-    <mergeCell ref="E6:E9"/>
-    <mergeCell ref="E10:E13"/>
-    <mergeCell ref="E18:E21"/>
-    <mergeCell ref="E14:E17"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="F26:F29"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="E22:E25"/>
-    <mergeCell ref="E26:E29"/>
-    <mergeCell ref="F18:F21"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="E34:E37"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="F14:F17"/>
-    <mergeCell ref="D14:D17"/>
-    <mergeCell ref="E38:E41"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="C34:C37"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="E30:E33"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="C26:C29"/>
-    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="D2:D5"/>
+    <mergeCell ref="F2:F5"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="F10:F13"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="F6:F9"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C12:C13"/>
     <mergeCell ref="A38:A41"/>
     <mergeCell ref="B38:B41"/>
     <mergeCell ref="D38:D41"/>
@@ -1690,22 +1670,36 @@
     <mergeCell ref="B30:B33"/>
     <mergeCell ref="D30:D33"/>
     <mergeCell ref="F30:F33"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="D2:D5"/>
-    <mergeCell ref="F2:F5"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="F10:F13"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="D6:D9"/>
-    <mergeCell ref="F6:F9"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="E34:E37"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="F14:F17"/>
+    <mergeCell ref="D14:D17"/>
+    <mergeCell ref="E38:E41"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="C34:C37"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="E30:E33"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="C26:C29"/>
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="F26:F29"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="E22:E25"/>
+    <mergeCell ref="E26:E29"/>
+    <mergeCell ref="F18:F21"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="E6:E9"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="E18:E21"/>
+    <mergeCell ref="E14:E17"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Información de usuario mejorada
</commit_message>
<xml_diff>
--- a/ToDo/Product Backlog.xlsx
+++ b/ToDo/Product Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minie\Desktop\UMA\Tercer Curso\2do cuatrimestre\Tecnologías de Aplicaciones Web\Trabajo en grupo\ArkhamMovies\ToDo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FFC1FE0-7967-443E-AAF5-2BD399C060A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A4F64D9-85F5-4A28-B431-F48311F1D54F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{391AEB77-1329-4C84-A561-AE54ADC33E64}"/>
   </bookViews>
@@ -362,9 +362,6 @@
     <t>Implementar la ordenación de películas según su popularidad.</t>
   </si>
   <si>
-    <t>José Luis</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Como </t>
     </r>
@@ -723,6 +720,9 @@
   <si>
     <t>Añadir porcentajes de creación en cada 
 clase/jsp</t>
+  </si>
+  <si>
+    <t>Alguien</t>
   </si>
 </sst>
 </file>
@@ -900,6 +900,75 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -909,86 +978,17 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1327,7 +1327,7 @@
   <dimension ref="A1:H61"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="H56" sqref="H56"/>
+      <selection activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1359,712 +1359,790 @@
         <v>4</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" s="18" t="s">
+      <c r="A2" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>25</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="H2" s="18" t="s">
-        <v>75</v>
+      <c r="H2" s="9" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
-      <c r="B3" s="19"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="13"/>
       <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="10"/>
-      <c r="H3" s="16"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="26"/>
+      <c r="H3" s="10"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
-      <c r="B4" s="19"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="13"/>
       <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="10"/>
-      <c r="H4" s="16"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="26"/>
+      <c r="H4" s="10"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
-      <c r="B5" s="20"/>
+      <c r="A5" s="11"/>
+      <c r="B5" s="14"/>
       <c r="C5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="20"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="11"/>
-      <c r="H5" s="17"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="27"/>
+      <c r="H5" s="11"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="10"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="26"/>
+      <c r="H7" s="10"/>
+    </row>
+    <row r="8" spans="1:8" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="10"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="13"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="26"/>
+      <c r="H8" s="10"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="11"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="27"/>
+      <c r="H9" s="11"/>
+    </row>
+    <row r="10" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="18" t="s">
+      <c r="B10" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E10" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="H6" s="18" t="s">
+      <c r="F10" s="25" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="10"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="26"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="10"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="13"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="26"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="11"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="27"/>
+    </row>
+    <row r="14" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="25" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="10"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="26"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="10"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="13"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="26"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="11"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="27"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="25" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="10"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="26"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="10"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="13"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="26"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="11"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="27"/>
+    </row>
+    <row r="22" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E22" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="10"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="13"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="7"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="10"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" s="13"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="7"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="11"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" s="14"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="8"/>
+    </row>
+    <row r="26" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26" s="9" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="10"/>
-      <c r="H7" s="16"/>
-    </row>
-    <row r="8" spans="1:8" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="19"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="10"/>
-      <c r="H8" s="16"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="11"/>
-      <c r="H9" s="17"/>
-    </row>
-    <row r="10" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="6" t="s">
+      <c r="E26" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="10"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="19"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="10"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
-      <c r="B13" s="20"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="11"/>
-    </row>
-    <row r="14" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="16"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="10"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="16"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="19"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="10"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="17"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="11"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B18" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="16"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="10"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="16"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="D20" s="19"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="10"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="17"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="11"/>
-    </row>
-    <row r="22" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="B22" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D22" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F22" s="24" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="16"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D23" s="19"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="25"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="16"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D24" s="19"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="25"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="17"/>
-      <c r="B25" s="20"/>
-      <c r="C25" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D25" s="20"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="26"/>
-    </row>
-    <row r="26" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="15" t="s">
+      <c r="F26" s="32" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="10"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="33"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="10"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="33"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="11"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="34"/>
+    </row>
+    <row r="30" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="B26" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="C26" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="D26" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F26" s="28" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="16"/>
-      <c r="B27" s="19"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="29"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="16"/>
-      <c r="B28" s="19"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="29"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="17"/>
-      <c r="B29" s="20"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="30"/>
-    </row>
-    <row r="30" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="B30" s="18" t="s">
+      <c r="B30" s="9" t="s">
         <v>15</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D30" s="18" t="s">
+      <c r="D30" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E30" s="21" t="s">
+      <c r="E30" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F30" s="28" t="s">
+      <c r="F30" s="32" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="16"/>
-      <c r="B31" s="19"/>
+      <c r="A31" s="10"/>
+      <c r="B31" s="13"/>
       <c r="C31" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D31" s="19"/>
-      <c r="E31" s="22"/>
-      <c r="F31" s="29"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="33"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="16"/>
-      <c r="B32" s="19"/>
+      <c r="A32" s="10"/>
+      <c r="B32" s="13"/>
       <c r="C32" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D32" s="19"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="29"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="33"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="17"/>
-      <c r="B33" s="20"/>
+      <c r="A33" s="11"/>
+      <c r="B33" s="14"/>
       <c r="C33" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D33" s="20"/>
-      <c r="E33" s="23"/>
-      <c r="F33" s="30"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="34"/>
     </row>
     <row r="34" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="15" t="s">
+      <c r="A34" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E34" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F34" s="32" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="10"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="33"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="10"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="33"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="11"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="34"/>
+    </row>
+    <row r="38" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="B34" s="18" t="s">
+      <c r="B38" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C34" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="D34" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="E34" s="21" t="s">
+      <c r="C38" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E38" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F34" s="28" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="16"/>
-      <c r="B35" s="19"/>
-      <c r="C35" s="16"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="22"/>
-      <c r="F35" s="29"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="16"/>
-      <c r="B36" s="19"/>
-      <c r="C36" s="16"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="22"/>
-      <c r="F36" s="29"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="17"/>
-      <c r="B37" s="20"/>
-      <c r="C37" s="17"/>
-      <c r="D37" s="20"/>
-      <c r="E37" s="23"/>
-      <c r="F37" s="30"/>
-    </row>
-    <row r="38" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="B38" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="C38" s="12" t="s">
+      <c r="F38" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="G38" s="4"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="10"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="22"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="10"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D38" s="18" t="s">
+      <c r="D40" s="13"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="22"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="11"/>
+      <c r="B41" s="14"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="23"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="D42" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E38" s="21" t="s">
+      <c r="E42" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F38" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="G38" s="4"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="16"/>
-      <c r="B39" s="19"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="19"/>
-      <c r="E39" s="22"/>
-      <c r="F39" s="32"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="16"/>
-      <c r="B40" s="19"/>
-      <c r="C40" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D40" s="19"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="32"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="17"/>
-      <c r="B41" s="20"/>
-      <c r="C41" s="17"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="23"/>
-      <c r="F41" s="33"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="15" t="s">
+      <c r="F42" s="25" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="10"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="26"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="10"/>
+      <c r="B44" s="13"/>
+      <c r="C44" s="16"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="26"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="11"/>
+      <c r="B45" s="14"/>
+      <c r="C45" s="17"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="20"/>
+      <c r="F45" s="27"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B46" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B42" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="C42" s="12" t="s">
+      <c r="C46" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E46" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="10"/>
+      <c r="B47" s="13"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="19"/>
+      <c r="F47" s="7"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="10"/>
+      <c r="B48" s="13"/>
+      <c r="C48" s="16"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="19"/>
+      <c r="F48" s="7"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="11"/>
+      <c r="B49" s="14"/>
+      <c r="C49" s="17"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="20"/>
+      <c r="F49" s="8"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C50" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="D50" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="D42" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="E42" s="21" t="s">
+      <c r="E50" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F42" s="9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="16"/>
-      <c r="B43" s="19"/>
-      <c r="C43" s="13"/>
-      <c r="D43" s="19"/>
-      <c r="E43" s="22"/>
-      <c r="F43" s="10"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="16"/>
-      <c r="B44" s="19"/>
-      <c r="C44" s="13"/>
-      <c r="D44" s="19"/>
-      <c r="E44" s="22"/>
-      <c r="F44" s="10"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="17"/>
-      <c r="B45" s="20"/>
-      <c r="C45" s="14"/>
-      <c r="D45" s="20"/>
-      <c r="E45" s="23"/>
-      <c r="F45" s="11"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="B46" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="C46" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="D46" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="E46" s="21" t="s">
+      <c r="F50" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="10"/>
+      <c r="B51" s="13"/>
+      <c r="C51" s="16"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="19"/>
+      <c r="F51" s="7"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="10"/>
+      <c r="B52" s="13"/>
+      <c r="C52" s="16"/>
+      <c r="D52" s="13"/>
+      <c r="E52" s="19"/>
+      <c r="F52" s="7"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="11"/>
+      <c r="B53" s="14"/>
+      <c r="C53" s="17"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="20"/>
+      <c r="F53" s="8"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C54" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="D54" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E54" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F46" s="24" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="16"/>
-      <c r="B47" s="19"/>
-      <c r="C47" s="13"/>
-      <c r="D47" s="19"/>
-      <c r="E47" s="22"/>
-      <c r="F47" s="25"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="16"/>
-      <c r="B48" s="19"/>
-      <c r="C48" s="13"/>
-      <c r="D48" s="19"/>
-      <c r="E48" s="22"/>
-      <c r="F48" s="25"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="17"/>
-      <c r="B49" s="20"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="20"/>
-      <c r="E49" s="23"/>
-      <c r="F49" s="26"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="B50" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="C50" s="15" t="s">
+      <c r="F54" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="10"/>
+      <c r="B55" s="13"/>
+      <c r="C55" s="16"/>
+      <c r="D55" s="13"/>
+      <c r="E55" s="19"/>
+      <c r="F55" s="7"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="10"/>
+      <c r="B56" s="13"/>
+      <c r="C56" s="16"/>
+      <c r="D56" s="13"/>
+      <c r="E56" s="19"/>
+      <c r="F56" s="7"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="11"/>
+      <c r="B57" s="14"/>
+      <c r="C57" s="17"/>
+      <c r="D57" s="14"/>
+      <c r="E57" s="20"/>
+      <c r="F57" s="8"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B58" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="D50" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="E50" s="21" t="s">
+      <c r="C58" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="D58" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E58" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F50" s="31" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="16"/>
-      <c r="B51" s="19"/>
-      <c r="C51" s="13"/>
-      <c r="D51" s="19"/>
-      <c r="E51" s="22"/>
-      <c r="F51" s="32"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="16"/>
-      <c r="B52" s="19"/>
-      <c r="C52" s="13"/>
-      <c r="D52" s="19"/>
-      <c r="E52" s="22"/>
-      <c r="F52" s="32"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="17"/>
-      <c r="B53" s="20"/>
-      <c r="C53" s="14"/>
-      <c r="D53" s="20"/>
-      <c r="E53" s="23"/>
-      <c r="F53" s="33"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="B54" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="C54" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="D54" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="E54" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F54" s="24" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="16"/>
-      <c r="B55" s="19"/>
-      <c r="C55" s="13"/>
-      <c r="D55" s="19"/>
-      <c r="E55" s="22"/>
-      <c r="F55" s="25"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="16"/>
-      <c r="B56" s="19"/>
-      <c r="C56" s="13"/>
-      <c r="D56" s="19"/>
-      <c r="E56" s="22"/>
-      <c r="F56" s="25"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="17"/>
-      <c r="B57" s="20"/>
-      <c r="C57" s="14"/>
-      <c r="D57" s="20"/>
-      <c r="E57" s="23"/>
-      <c r="F57" s="26"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="B58" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="C58" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="D58" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="E58" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F58" s="24" t="s">
-        <v>57</v>
+      <c r="F58" s="6" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="16"/>
-      <c r="B59" s="19"/>
-      <c r="C59" s="13"/>
-      <c r="D59" s="19"/>
-      <c r="E59" s="22"/>
-      <c r="F59" s="25"/>
+      <c r="A59" s="10"/>
+      <c r="B59" s="13"/>
+      <c r="C59" s="16"/>
+      <c r="D59" s="13"/>
+      <c r="E59" s="19"/>
+      <c r="F59" s="7"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="16"/>
-      <c r="B60" s="19"/>
-      <c r="C60" s="13"/>
-      <c r="D60" s="19"/>
-      <c r="E60" s="22"/>
-      <c r="F60" s="25"/>
+      <c r="A60" s="10"/>
+      <c r="B60" s="13"/>
+      <c r="C60" s="16"/>
+      <c r="D60" s="13"/>
+      <c r="E60" s="19"/>
+      <c r="F60" s="7"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="17"/>
-      <c r="B61" s="20"/>
-      <c r="C61" s="14"/>
-      <c r="D61" s="20"/>
-      <c r="E61" s="23"/>
-      <c r="F61" s="26"/>
+      <c r="A61" s="11"/>
+      <c r="B61" s="14"/>
+      <c r="C61" s="17"/>
+      <c r="D61" s="14"/>
+      <c r="E61" s="20"/>
+      <c r="F61" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="94">
+    <mergeCell ref="F14:F17"/>
+    <mergeCell ref="D14:D17"/>
+    <mergeCell ref="F42:F45"/>
+    <mergeCell ref="C42:C45"/>
+    <mergeCell ref="A46:A49"/>
+    <mergeCell ref="B46:B49"/>
+    <mergeCell ref="C46:C49"/>
+    <mergeCell ref="D46:D49"/>
+    <mergeCell ref="E46:E49"/>
+    <mergeCell ref="F46:F49"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="B42:B45"/>
+    <mergeCell ref="D42:D45"/>
+    <mergeCell ref="E42:E45"/>
+    <mergeCell ref="E38:E41"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="C34:C37"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="E30:E33"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="C26:C29"/>
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="E18:E21"/>
+    <mergeCell ref="E14:E17"/>
+    <mergeCell ref="F26:F29"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="E22:E25"/>
+    <mergeCell ref="E26:E29"/>
+    <mergeCell ref="F18:F21"/>
+    <mergeCell ref="F38:F41"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="D22:D25"/>
+    <mergeCell ref="F22:F25"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="F34:F37"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="F30:F33"/>
+    <mergeCell ref="E34:E37"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="F2:F5"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="F10:F13"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="F6:F9"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="E6:E9"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="B50:B53"/>
+    <mergeCell ref="C50:C53"/>
+    <mergeCell ref="D50:D53"/>
+    <mergeCell ref="E50:E53"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="D2:D5"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="D38:D41"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="B18:B21"/>
     <mergeCell ref="F58:F61"/>
     <mergeCell ref="H2:H5"/>
     <mergeCell ref="H6:H9"/>
@@ -2081,84 +2159,6 @@
     <mergeCell ref="E54:E57"/>
     <mergeCell ref="F54:F57"/>
     <mergeCell ref="A50:A53"/>
-    <mergeCell ref="B50:B53"/>
-    <mergeCell ref="C50:C53"/>
-    <mergeCell ref="D50:D53"/>
-    <mergeCell ref="E50:E53"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="D2:D5"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="B38:B41"/>
-    <mergeCell ref="D38:D41"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="F2:F5"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="F10:F13"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="D6:D9"/>
-    <mergeCell ref="F6:F9"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="E2:E5"/>
-    <mergeCell ref="E6:E9"/>
-    <mergeCell ref="E10:E13"/>
-    <mergeCell ref="F38:F41"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="D22:D25"/>
-    <mergeCell ref="F22:F25"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="F34:F37"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="F30:F33"/>
-    <mergeCell ref="E34:E37"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="F26:F29"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="E22:E25"/>
-    <mergeCell ref="E26:E29"/>
-    <mergeCell ref="F18:F21"/>
-    <mergeCell ref="E38:E41"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="C34:C37"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="E30:E33"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="C26:C29"/>
-    <mergeCell ref="D18:D21"/>
-    <mergeCell ref="E18:E21"/>
-    <mergeCell ref="E14:E17"/>
-    <mergeCell ref="F42:F45"/>
-    <mergeCell ref="C42:C45"/>
-    <mergeCell ref="A46:A49"/>
-    <mergeCell ref="B46:B49"/>
-    <mergeCell ref="C46:C49"/>
-    <mergeCell ref="D46:D49"/>
-    <mergeCell ref="E46:E49"/>
-    <mergeCell ref="F46:F49"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="B42:B45"/>
-    <mergeCell ref="D42:D45"/>
-    <mergeCell ref="E42:E45"/>
-    <mergeCell ref="F14:F17"/>
-    <mergeCell ref="D14:D17"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Estadisticas en el perfil
Borrado el anterior boton de estadísticas
</commit_message>
<xml_diff>
--- a/ToDo/Product Backlog.xlsx
+++ b/ToDo/Product Backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juana\Escritorio\UNI\Tercero\Segundo Cuatrimestre\TaW\ArkhamMovies\ToDo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minie\Desktop\UMA\Tercer Curso\2do cuatrimestre\Tecnologías de Aplicaciones Web\Trabajo en grupo\ArkhamMovies\ToDo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE1BAA38-CFFD-40A6-A161-B545FE36227C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C38FC35A-DE8E-4192-9FA3-4CD3FC23EDCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{391AEB77-1329-4C84-A561-AE54ADC33E64}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{391AEB77-1329-4C84-A561-AE54ADC33E64}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="86">
   <si>
     <t>ID</t>
   </si>
@@ -817,6 +817,9 @@
   </si>
   <si>
     <t>Añadir listas en personas y personajes en las que aparezcan los que aparecen en tus peliculas con like</t>
+  </si>
+  <si>
+    <t>US18</t>
   </si>
 </sst>
 </file>
@@ -994,6 +997,81 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1003,86 +1081,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1420,20 +1423,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D14C92F-3F4B-401B-9B84-B21C184BF8CD}">
   <dimension ref="A1:H73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G61" sqref="G61"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="34.109375" customWidth="1"/>
-    <col min="3" max="3" width="66.88671875" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" customWidth="1"/>
-    <col min="6" max="6" width="13.88671875" customWidth="1"/>
-    <col min="8" max="8" width="33.5546875" customWidth="1"/>
+    <col min="2" max="2" width="34.140625" customWidth="1"/>
+    <col min="3" max="3" width="66.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" customWidth="1"/>
+    <col min="8" max="8" width="33.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1456,911 +1459,859 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="15" t="s">
         <v>25</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="35" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="10"/>
-      <c r="B3" s="13"/>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="13"/>
+      <c r="B3" s="16"/>
       <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="26"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="7"/>
       <c r="H3" s="10"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="10"/>
-      <c r="B4" s="13"/>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="13"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="26"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="7"/>
       <c r="H4" s="10"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="11"/>
-      <c r="B5" s="14"/>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="14"/>
+      <c r="B5" s="17"/>
       <c r="C5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="27"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="8"/>
       <c r="H5" s="11"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="29" t="s">
+      <c r="E6" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="25" t="s">
+      <c r="F6" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="H6" s="15" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="10"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="26"/>
-      <c r="H7" s="10"/>
-    </row>
-    <row r="8" spans="1:8" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="10"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="12" t="s">
+    <row r="7" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="13"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="7"/>
+      <c r="H7" s="13"/>
+    </row>
+    <row r="8" spans="1:8" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="13"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="26"/>
-      <c r="H8" s="10"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="11"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="27"/>
-      <c r="H9" s="11"/>
-    </row>
-    <row r="10" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
+      <c r="D8" s="16"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="7"/>
+      <c r="H8" s="13"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="14"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="8"/>
+      <c r="H9" s="14"/>
+    </row>
+    <row r="10" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="29" t="s">
+      <c r="E10" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="25" t="s">
+      <c r="F10" s="6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="10"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="26"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="10"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="12" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="13"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="7"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="13"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="26"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="11"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="27"/>
-    </row>
-    <row r="14" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="9" t="s">
+      <c r="D12" s="16"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="8"/>
+    </row>
+    <row r="14" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="21" t="s">
+      <c r="C14" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="29" t="s">
+      <c r="E14" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="25" t="s">
+      <c r="F14" s="6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="10"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="26"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="10"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="21" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="13"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="7"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="13"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="13"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="26"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="11"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="27"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="9" t="s">
+      <c r="D16" s="16"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="7"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="14"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="8"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="21" t="s">
+      <c r="C18" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="E18" s="29" t="s">
+      <c r="E18" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="F18" s="25" t="s">
+      <c r="F18" s="6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="10"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="26"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="10"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="21" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="13"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="7"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="13"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="13"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="26"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="11"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="35"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="27"/>
-    </row>
-    <row r="22" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="9" t="s">
+      <c r="D20" s="16"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="7"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="14"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="8"/>
+    </row>
+    <row r="22" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="15" t="s">
         <v>39</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="D22" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="E22" s="29" t="s">
+      <c r="E22" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="F22" s="18" t="s">
+      <c r="F22" s="21" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="10"/>
-      <c r="B23" s="13"/>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="13"/>
+      <c r="B23" s="16"/>
       <c r="C23" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="13"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="19"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="10"/>
-      <c r="B24" s="13"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="22"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="13"/>
+      <c r="B24" s="16"/>
       <c r="C24" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D24" s="13"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="19"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="11"/>
-      <c r="B25" s="14"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="22"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="14"/>
+      <c r="B25" s="17"/>
       <c r="C25" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="14"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="20"/>
-    </row>
-    <row r="26" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="9" t="s">
+      <c r="D25" s="17"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="23"/>
+    </row>
+    <row r="26" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="B26" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C26" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D26" s="12" t="s">
+      <c r="D26" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="E26" s="29" t="s">
+      <c r="E26" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="F26" s="6" t="s">
+      <c r="F26" s="31" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="10"/>
-      <c r="B27" s="13"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="7"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="10"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="7"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="11"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="8"/>
-    </row>
-    <row r="30" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="9" t="s">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="13"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="32"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="13"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="32"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="14"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="33"/>
+    </row>
+    <row r="30" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="15" t="s">
         <v>15</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D30" s="12" t="s">
+      <c r="D30" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E30" s="15" t="s">
+      <c r="E30" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F30" s="6" t="s">
+      <c r="F30" s="31" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="10"/>
-      <c r="B31" s="13"/>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="13"/>
+      <c r="B31" s="16"/>
       <c r="C31" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D31" s="13"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="7"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="10"/>
-      <c r="B32" s="13"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="32"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="13"/>
+      <c r="B32" s="16"/>
       <c r="C32" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D32" s="13"/>
-      <c r="E32" s="16"/>
-      <c r="F32" s="7"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="11"/>
-      <c r="B33" s="14"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="32"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="14"/>
+      <c r="B33" s="17"/>
       <c r="C33" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D33" s="14"/>
-      <c r="E33" s="17"/>
-      <c r="F33" s="8"/>
-    </row>
-    <row r="34" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="9" t="s">
+      <c r="D33" s="17"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="33"/>
+    </row>
+    <row r="34" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="B34" s="12" t="s">
+      <c r="B34" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="9" t="s">
+      <c r="C34" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D34" s="12" t="s">
+      <c r="D34" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="E34" s="15" t="s">
+      <c r="E34" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F34" s="6" t="s">
+      <c r="F34" s="31" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="10"/>
-      <c r="B35" s="13"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="7"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="10"/>
-      <c r="B36" s="13"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="16"/>
-      <c r="F36" s="7"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="11"/>
-      <c r="B37" s="14"/>
-      <c r="C37" s="11"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="17"/>
-      <c r="F37" s="8"/>
-    </row>
-    <row r="38" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="9" t="s">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="13"/>
+      <c r="B35" s="16"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="32"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="13"/>
+      <c r="B36" s="16"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="32"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="14"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="33"/>
+    </row>
+    <row r="38" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="B38" s="12" t="s">
+      <c r="B38" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C38" s="21" t="s">
+      <c r="C38" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D38" s="12" t="s">
+      <c r="D38" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="E38" s="15" t="s">
+      <c r="E38" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F38" s="32" t="s">
+      <c r="F38" s="28" t="s">
         <v>57</v>
       </c>
       <c r="G38" s="4"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="10"/>
-      <c r="B39" s="13"/>
-      <c r="C39" s="23"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="16"/>
-      <c r="F39" s="33"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="10"/>
-      <c r="B40" s="13"/>
-      <c r="C40" s="9" t="s">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="13"/>
+      <c r="B39" s="16"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="29"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="13"/>
+      <c r="B40" s="16"/>
+      <c r="C40" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D40" s="13"/>
-      <c r="E40" s="16"/>
-      <c r="F40" s="33"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="11"/>
-      <c r="B41" s="14"/>
-      <c r="C41" s="11"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="17"/>
-      <c r="F41" s="34"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="9" t="s">
+      <c r="D40" s="16"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="29"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="14"/>
+      <c r="B41" s="17"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="30"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="B42" s="12" t="s">
+      <c r="B42" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="C42" s="21" t="s">
+      <c r="C42" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D42" s="12" t="s">
+      <c r="D42" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="E42" s="15" t="s">
+      <c r="E42" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F42" s="25" t="s">
+      <c r="F42" s="6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="10"/>
-      <c r="B43" s="13"/>
-      <c r="C43" s="22"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="16"/>
-      <c r="F43" s="26"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="10"/>
-      <c r="B44" s="13"/>
-      <c r="C44" s="22"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="16"/>
-      <c r="F44" s="26"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="11"/>
-      <c r="B45" s="14"/>
-      <c r="C45" s="23"/>
-      <c r="D45" s="14"/>
-      <c r="E45" s="17"/>
-      <c r="F45" s="27"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="9" t="s">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="13"/>
+      <c r="B43" s="16"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="7"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="13"/>
+      <c r="B44" s="16"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="16"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="7"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="14"/>
+      <c r="B45" s="17"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="17"/>
+      <c r="E45" s="20"/>
+      <c r="F45" s="8"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="B46" s="12" t="s">
+      <c r="B46" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="C46" s="21" t="s">
+      <c r="C46" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="D46" s="12" t="s">
+      <c r="D46" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="E46" s="15" t="s">
+      <c r="E46" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F46" s="18" t="s">
+      <c r="F46" s="21" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="10"/>
-      <c r="B47" s="13"/>
-      <c r="C47" s="22"/>
-      <c r="D47" s="13"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="19"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="10"/>
-      <c r="B48" s="13"/>
-      <c r="C48" s="22"/>
-      <c r="D48" s="13"/>
-      <c r="E48" s="16"/>
-      <c r="F48" s="19"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" s="11"/>
-      <c r="B49" s="14"/>
-      <c r="C49" s="23"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="17"/>
-      <c r="F49" s="20"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" s="9" t="s">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="13"/>
+      <c r="B47" s="16"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="19"/>
+      <c r="F47" s="22"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="13"/>
+      <c r="B48" s="16"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="16"/>
+      <c r="E48" s="19"/>
+      <c r="F48" s="22"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="14"/>
+      <c r="B49" s="17"/>
+      <c r="C49" s="11"/>
+      <c r="D49" s="17"/>
+      <c r="E49" s="20"/>
+      <c r="F49" s="23"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="B50" s="12" t="s">
+      <c r="B50" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="C50" s="21" t="s">
+      <c r="C50" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D50" s="12" t="s">
+      <c r="D50" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="E50" s="15" t="s">
+      <c r="E50" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F50" s="18" t="s">
+      <c r="F50" s="21" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="10"/>
-      <c r="B51" s="13"/>
-      <c r="C51" s="22"/>
-      <c r="D51" s="13"/>
-      <c r="E51" s="16"/>
-      <c r="F51" s="19"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" s="10"/>
-      <c r="B52" s="13"/>
-      <c r="C52" s="22"/>
-      <c r="D52" s="13"/>
-      <c r="E52" s="16"/>
-      <c r="F52" s="19"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" s="11"/>
-      <c r="B53" s="14"/>
-      <c r="C53" s="23"/>
-      <c r="D53" s="14"/>
-      <c r="E53" s="17"/>
-      <c r="F53" s="20"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" s="9" t="s">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="13"/>
+      <c r="B51" s="16"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="16"/>
+      <c r="E51" s="19"/>
+      <c r="F51" s="22"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="13"/>
+      <c r="B52" s="16"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="16"/>
+      <c r="E52" s="19"/>
+      <c r="F52" s="22"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="14"/>
+      <c r="B53" s="17"/>
+      <c r="C53" s="11"/>
+      <c r="D53" s="17"/>
+      <c r="E53" s="20"/>
+      <c r="F53" s="23"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="B54" s="12" t="s">
+      <c r="B54" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="C54" s="24" t="s">
+      <c r="C54" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="D54" s="12" t="s">
+      <c r="D54" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="E54" s="15" t="s">
+      <c r="E54" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F54" s="18" t="s">
+      <c r="F54" s="21" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" s="10"/>
-      <c r="B55" s="13"/>
-      <c r="C55" s="22"/>
-      <c r="D55" s="13"/>
-      <c r="E55" s="16"/>
-      <c r="F55" s="19"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" s="10"/>
-      <c r="B56" s="13"/>
-      <c r="C56" s="22"/>
-      <c r="D56" s="13"/>
-      <c r="E56" s="16"/>
-      <c r="F56" s="19"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A57" s="11"/>
-      <c r="B57" s="14"/>
-      <c r="C57" s="23"/>
-      <c r="D57" s="14"/>
-      <c r="E57" s="17"/>
-      <c r="F57" s="20"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58" s="9" t="s">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="13"/>
+      <c r="B55" s="16"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="16"/>
+      <c r="E55" s="19"/>
+      <c r="F55" s="22"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="13"/>
+      <c r="B56" s="16"/>
+      <c r="C56" s="10"/>
+      <c r="D56" s="16"/>
+      <c r="E56" s="19"/>
+      <c r="F56" s="22"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="14"/>
+      <c r="B57" s="17"/>
+      <c r="C57" s="11"/>
+      <c r="D57" s="17"/>
+      <c r="E57" s="20"/>
+      <c r="F57" s="23"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="B58" s="12" t="s">
+      <c r="B58" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="C58" s="21" t="s">
+      <c r="C58" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="D58" s="12" t="s">
+      <c r="D58" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="E58" s="15" t="s">
+      <c r="E58" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F58" s="18" t="s">
+      <c r="F58" s="21" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" s="10"/>
-      <c r="B59" s="13"/>
-      <c r="C59" s="22"/>
-      <c r="D59" s="13"/>
-      <c r="E59" s="16"/>
-      <c r="F59" s="19"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A60" s="10"/>
-      <c r="B60" s="13"/>
-      <c r="C60" s="22"/>
-      <c r="D60" s="13"/>
-      <c r="E60" s="16"/>
-      <c r="F60" s="19"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A61" s="11"/>
-      <c r="B61" s="14"/>
-      <c r="C61" s="23"/>
-      <c r="D61" s="14"/>
-      <c r="E61" s="17"/>
-      <c r="F61" s="20"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" s="9" t="s">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="13"/>
+      <c r="B59" s="16"/>
+      <c r="C59" s="10"/>
+      <c r="D59" s="16"/>
+      <c r="E59" s="19"/>
+      <c r="F59" s="22"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="13"/>
+      <c r="B60" s="16"/>
+      <c r="C60" s="10"/>
+      <c r="D60" s="16"/>
+      <c r="E60" s="19"/>
+      <c r="F60" s="22"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="14"/>
+      <c r="B61" s="17"/>
+      <c r="C61" s="11"/>
+      <c r="D61" s="17"/>
+      <c r="E61" s="20"/>
+      <c r="F61" s="23"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="B62" s="12" t="s">
+      <c r="B62" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="C62" s="24" t="s">
+      <c r="C62" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="D62" s="12" t="s">
+      <c r="D62" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="E62" s="15" t="s">
+      <c r="E62" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F62" s="18" t="s">
+      <c r="F62" s="21" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A63" s="10"/>
-      <c r="B63" s="13"/>
-      <c r="C63" s="22"/>
-      <c r="D63" s="13"/>
-      <c r="E63" s="16"/>
-      <c r="F63" s="19"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A64" s="10"/>
-      <c r="B64" s="13"/>
-      <c r="C64" s="22"/>
-      <c r="D64" s="13"/>
-      <c r="E64" s="16"/>
-      <c r="F64" s="19"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A65" s="11"/>
-      <c r="B65" s="14"/>
-      <c r="C65" s="23"/>
-      <c r="D65" s="14"/>
-      <c r="E65" s="17"/>
-      <c r="F65" s="20"/>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A66" s="9" t="s">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="13"/>
+      <c r="B63" s="16"/>
+      <c r="C63" s="10"/>
+      <c r="D63" s="16"/>
+      <c r="E63" s="19"/>
+      <c r="F63" s="22"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="13"/>
+      <c r="B64" s="16"/>
+      <c r="C64" s="10"/>
+      <c r="D64" s="16"/>
+      <c r="E64" s="19"/>
+      <c r="F64" s="22"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="14"/>
+      <c r="B65" s="17"/>
+      <c r="C65" s="11"/>
+      <c r="D65" s="17"/>
+      <c r="E65" s="20"/>
+      <c r="F65" s="23"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B66" s="12" t="s">
+      <c r="B66" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="C66" s="12" t="s">
+      <c r="C66" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="D66" s="12" t="s">
+      <c r="D66" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="E66" s="15" t="s">
+      <c r="E66" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F66" s="6" t="s">
+      <c r="F66" s="21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="13"/>
+      <c r="B67" s="16"/>
+      <c r="C67" s="10"/>
+      <c r="D67" s="16"/>
+      <c r="E67" s="19"/>
+      <c r="F67" s="22"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="13"/>
+      <c r="B68" s="16"/>
+      <c r="C68" s="10"/>
+      <c r="D68" s="16"/>
+      <c r="E68" s="19"/>
+      <c r="F68" s="22"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="14"/>
+      <c r="B69" s="17"/>
+      <c r="C69" s="11"/>
+      <c r="D69" s="17"/>
+      <c r="E69" s="20"/>
+      <c r="F69" s="23"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B70" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C70" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="D70" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E70" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F70" s="31" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A67" s="10"/>
-      <c r="B67" s="13"/>
-      <c r="C67" s="10"/>
-      <c r="D67" s="13"/>
-      <c r="E67" s="16"/>
-      <c r="F67" s="7"/>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A68" s="10"/>
-      <c r="B68" s="13"/>
-      <c r="C68" s="10"/>
-      <c r="D68" s="13"/>
-      <c r="E68" s="16"/>
-      <c r="F68" s="7"/>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A69" s="11"/>
-      <c r="B69" s="14"/>
-      <c r="C69" s="11"/>
-      <c r="D69" s="14"/>
-      <c r="E69" s="17"/>
-      <c r="F69" s="8"/>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A70" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="B70" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="C70" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="D70" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="E70" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="F70" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A71" s="10"/>
-      <c r="B71" s="13"/>
-      <c r="C71" s="10"/>
-      <c r="D71" s="13"/>
-      <c r="E71" s="16"/>
-      <c r="F71" s="7"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A72" s="10"/>
-      <c r="B72" s="13"/>
-      <c r="C72" s="10"/>
-      <c r="D72" s="13"/>
-      <c r="E72" s="16"/>
-      <c r="F72" s="7"/>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A73" s="11"/>
-      <c r="B73" s="14"/>
-      <c r="C73" s="11"/>
-      <c r="D73" s="14"/>
-      <c r="E73" s="17"/>
-      <c r="F73" s="8"/>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="13"/>
+      <c r="B71" s="16"/>
+      <c r="C71" s="13"/>
+      <c r="D71" s="16"/>
+      <c r="E71" s="19"/>
+      <c r="F71" s="32"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="13"/>
+      <c r="B72" s="16"/>
+      <c r="C72" s="13"/>
+      <c r="D72" s="16"/>
+      <c r="E72" s="19"/>
+      <c r="F72" s="32"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="14"/>
+      <c r="B73" s="17"/>
+      <c r="C73" s="14"/>
+      <c r="D73" s="17"/>
+      <c r="E73" s="20"/>
+      <c r="F73" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="112">
-    <mergeCell ref="F42:F45"/>
-    <mergeCell ref="C42:C45"/>
-    <mergeCell ref="A46:A49"/>
-    <mergeCell ref="B46:B49"/>
-    <mergeCell ref="C46:C49"/>
-    <mergeCell ref="D46:D49"/>
-    <mergeCell ref="E46:E49"/>
-    <mergeCell ref="F46:F49"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="B42:B45"/>
-    <mergeCell ref="D42:D45"/>
-    <mergeCell ref="E42:E45"/>
-    <mergeCell ref="F18:F21"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="C34:C37"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="E30:E33"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="C26:C29"/>
-    <mergeCell ref="D18:D21"/>
-    <mergeCell ref="E18:E21"/>
-    <mergeCell ref="E14:E17"/>
-    <mergeCell ref="F14:F17"/>
-    <mergeCell ref="D14:D17"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="F38:F41"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="D22:D25"/>
-    <mergeCell ref="F22:F25"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="F34:F37"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="F30:F33"/>
-    <mergeCell ref="E34:E37"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="F26:F29"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="E22:E25"/>
-    <mergeCell ref="E26:E29"/>
-    <mergeCell ref="E38:E41"/>
-    <mergeCell ref="B38:B41"/>
-    <mergeCell ref="D38:D41"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="F2:F5"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="F10:F13"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="D6:D9"/>
-    <mergeCell ref="F6:F9"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="E2:E5"/>
-    <mergeCell ref="E6:E9"/>
-    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="F70:F73"/>
+    <mergeCell ref="A70:A73"/>
+    <mergeCell ref="B70:B73"/>
+    <mergeCell ref="C70:C73"/>
+    <mergeCell ref="D70:D73"/>
+    <mergeCell ref="E70:E73"/>
+    <mergeCell ref="F62:F65"/>
+    <mergeCell ref="A66:A69"/>
+    <mergeCell ref="B66:B69"/>
+    <mergeCell ref="C66:C69"/>
+    <mergeCell ref="D66:D69"/>
+    <mergeCell ref="E66:E69"/>
+    <mergeCell ref="F66:F69"/>
+    <mergeCell ref="A62:A65"/>
+    <mergeCell ref="B62:B65"/>
+    <mergeCell ref="C62:C65"/>
+    <mergeCell ref="D62:D65"/>
+    <mergeCell ref="E62:E65"/>
     <mergeCell ref="F58:F61"/>
     <mergeCell ref="H2:H5"/>
     <mergeCell ref="H6:H9"/>
@@ -2385,24 +2336,76 @@
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="D2:D5"/>
     <mergeCell ref="A38:A41"/>
-    <mergeCell ref="F70:F73"/>
-    <mergeCell ref="A70:A73"/>
-    <mergeCell ref="B70:B73"/>
-    <mergeCell ref="C70:C73"/>
-    <mergeCell ref="D70:D73"/>
-    <mergeCell ref="E70:E73"/>
-    <mergeCell ref="F62:F65"/>
-    <mergeCell ref="A66:A69"/>
-    <mergeCell ref="B66:B69"/>
-    <mergeCell ref="C66:C69"/>
-    <mergeCell ref="D66:D69"/>
-    <mergeCell ref="E66:E69"/>
-    <mergeCell ref="F66:F69"/>
-    <mergeCell ref="A62:A65"/>
-    <mergeCell ref="B62:B65"/>
-    <mergeCell ref="C62:C65"/>
-    <mergeCell ref="D62:D65"/>
-    <mergeCell ref="E62:E65"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="F2:F5"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="F10:F13"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="F6:F9"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="E6:E9"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="F38:F41"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="D22:D25"/>
+    <mergeCell ref="F22:F25"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="F34:F37"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="F30:F33"/>
+    <mergeCell ref="E34:E37"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="F26:F29"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="E22:E25"/>
+    <mergeCell ref="E26:E29"/>
+    <mergeCell ref="E38:E41"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="D38:D41"/>
+    <mergeCell ref="F18:F21"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="C34:C37"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="E30:E33"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="C26:C29"/>
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="E18:E21"/>
+    <mergeCell ref="E14:E17"/>
+    <mergeCell ref="F14:F17"/>
+    <mergeCell ref="D14:D17"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="F42:F45"/>
+    <mergeCell ref="C42:C45"/>
+    <mergeCell ref="A46:A49"/>
+    <mergeCell ref="B46:B49"/>
+    <mergeCell ref="C46:C49"/>
+    <mergeCell ref="D46:D49"/>
+    <mergeCell ref="E46:E49"/>
+    <mergeCell ref="F46:F49"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="B42:B45"/>
+    <mergeCell ref="D42:D45"/>
+    <mergeCell ref="E42:E45"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Salen los personajes de peliculas que te gustan
</commit_message>
<xml_diff>
--- a/ToDo/Product Backlog.xlsx
+++ b/ToDo/Product Backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minie\Desktop\UMA\Tercer Curso\2do cuatrimestre\Tecnologías de Aplicaciones Web\Trabajo en grupo\ArkhamMovies\ToDo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juana\Escritorio\UNI\Tercero\Segundo Cuatrimestre\TaW\ArkhamMovies\ToDo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C38FC35A-DE8E-4192-9FA3-4CD3FC23EDCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C31F6AC-6C9F-47CD-BFB4-EB13977ED648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{391AEB77-1329-4C84-A561-AE54ADC33E64}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{391AEB77-1329-4C84-A561-AE54ADC33E64}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -816,10 +816,10 @@
     </r>
   </si>
   <si>
-    <t>Añadir listas en personas y personajes en las que aparezcan los que aparecen en tus peliculas con like</t>
-  </si>
-  <si>
     <t>US18</t>
+  </si>
+  <si>
+    <t>Añadir listas en personas y personajes en las que aparezcan los que aparecen en tus peliculas con like (hecha la parte de personajes)</t>
   </si>
 </sst>
 </file>
@@ -997,6 +997,63 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1006,86 +1063,29 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1423,20 +1423,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D14C92F-3F4B-401B-9B84-B21C184BF8CD}">
   <dimension ref="A1:H73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="34.140625" customWidth="1"/>
-    <col min="3" max="3" width="66.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" customWidth="1"/>
-    <col min="8" max="8" width="33.5703125" customWidth="1"/>
+    <col min="2" max="2" width="34.109375" customWidth="1"/>
+    <col min="3" max="3" width="66.88671875" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" customWidth="1"/>
+    <col min="8" max="8" width="33.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1459,859 +1459,911 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="H2" s="35" t="s">
+      <c r="H2" s="21" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="16"/>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="10"/>
+      <c r="B3" s="13"/>
       <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="7"/>
-      <c r="H3" s="10"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="16"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="26"/>
+      <c r="H3" s="22"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="10"/>
+      <c r="B4" s="13"/>
       <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="7"/>
-      <c r="H4" s="10"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="17"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="26"/>
+      <c r="H4" s="22"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="11"/>
+      <c r="B5" s="14"/>
       <c r="C5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="17"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="8"/>
-      <c r="H5" s="11"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+      <c r="D5" s="14"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="27"/>
+      <c r="H5" s="23"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="25" t="s">
+      <c r="E6" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="H6" s="15" t="s">
+      <c r="H6" s="12" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="7"/>
-      <c r="H7" s="13"/>
-    </row>
-    <row r="8" spans="1:8" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="15" t="s">
+    <row r="7" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="10"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="26"/>
+      <c r="H7" s="10"/>
+    </row>
+    <row r="8" spans="1:8" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="10"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="7"/>
-      <c r="H8" s="13"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="8"/>
-      <c r="H9" s="14"/>
-    </row>
-    <row r="10" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+      <c r="D8" s="13"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="26"/>
+      <c r="H8" s="10"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="11"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="27"/>
+      <c r="H9" s="11"/>
+    </row>
+    <row r="10" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="25" t="s">
+      <c r="E10" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="25" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="7"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="15" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="10"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="26"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="10"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="16"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="7"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="8"/>
-    </row>
-    <row r="14" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="12" t="s">
+      <c r="D12" s="13"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="26"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="11"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="27"/>
+    </row>
+    <row r="14" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="25" t="s">
+      <c r="E14" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="25" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="7"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="9" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="10"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="26"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="10"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="16"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="7"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="8"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
+      <c r="D16" s="13"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="26"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="11"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="27"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="E18" s="25" t="s">
+      <c r="E18" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="25" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="7"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="9" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="10"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="26"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="10"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="16"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="7"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="8"/>
-    </row>
-    <row r="22" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="12" t="s">
+      <c r="D20" s="13"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="26"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="11"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="27"/>
+    </row>
+    <row r="22" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="12" t="s">
         <v>39</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D22" s="15" t="s">
+      <c r="D22" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E22" s="25" t="s">
+      <c r="E22" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="F22" s="21" t="s">
+      <c r="F22" s="18" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="13"/>
-      <c r="B23" s="16"/>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="10"/>
+      <c r="B23" s="13"/>
       <c r="C23" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="16"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="22"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="13"/>
-      <c r="B24" s="16"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="19"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="10"/>
+      <c r="B24" s="13"/>
       <c r="C24" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D24" s="16"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="22"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="14"/>
-      <c r="B25" s="17"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="19"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="11"/>
+      <c r="B25" s="14"/>
       <c r="C25" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="17"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="23"/>
-    </row>
-    <row r="26" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
+      <c r="D25" s="14"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="20"/>
+    </row>
+    <row r="26" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C26" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D26" s="15" t="s">
+      <c r="D26" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="E26" s="25" t="s">
+      <c r="E26" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="F26" s="31" t="s">
+      <c r="F26" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="13"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="32"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="13"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="32"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="14"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="33"/>
-    </row>
-    <row r="30" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="12" t="s">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="10"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="7"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="10"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="7"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="11"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="8"/>
+    </row>
+    <row r="30" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D30" s="15" t="s">
+      <c r="D30" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E30" s="18" t="s">
+      <c r="E30" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F30" s="31" t="s">
+      <c r="F30" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="13"/>
-      <c r="B31" s="16"/>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="10"/>
+      <c r="B31" s="13"/>
       <c r="C31" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D31" s="16"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="32"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="13"/>
-      <c r="B32" s="16"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="7"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="10"/>
+      <c r="B32" s="13"/>
       <c r="C32" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D32" s="16"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="32"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="14"/>
-      <c r="B33" s="17"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="7"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="11"/>
+      <c r="B33" s="14"/>
       <c r="C33" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D33" s="17"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="33"/>
-    </row>
-    <row r="34" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="12" t="s">
+      <c r="D33" s="14"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="8"/>
+    </row>
+    <row r="34" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B34" s="15" t="s">
+      <c r="B34" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="12" t="s">
+      <c r="C34" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="D34" s="15" t="s">
+      <c r="D34" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="E34" s="18" t="s">
+      <c r="E34" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F34" s="31" t="s">
+      <c r="F34" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="13"/>
-      <c r="B35" s="16"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="32"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="13"/>
-      <c r="B36" s="16"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="19"/>
-      <c r="F36" s="32"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="14"/>
-      <c r="B37" s="17"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="17"/>
-      <c r="E37" s="20"/>
-      <c r="F37" s="33"/>
-    </row>
-    <row r="38" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="12" t="s">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="10"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="7"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="10"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="7"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="11"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="23"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="8"/>
+    </row>
+    <row r="38" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B38" s="15" t="s">
+      <c r="B38" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C38" s="9" t="s">
+      <c r="C38" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="D38" s="15" t="s">
+      <c r="D38" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E38" s="18" t="s">
+      <c r="E38" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F38" s="28" t="s">
+      <c r="F38" s="32" t="s">
         <v>57</v>
       </c>
       <c r="G38" s="4"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="13"/>
-      <c r="B39" s="16"/>
-      <c r="C39" s="11"/>
-      <c r="D39" s="16"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="29"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="13"/>
-      <c r="B40" s="16"/>
-      <c r="C40" s="12" t="s">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" s="10"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="23"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="33"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" s="10"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D40" s="16"/>
-      <c r="E40" s="19"/>
-      <c r="F40" s="29"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="14"/>
-      <c r="B41" s="17"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="17"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="30"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="12" t="s">
+      <c r="D40" s="13"/>
+      <c r="E40" s="16"/>
+      <c r="F40" s="33"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" s="11"/>
+      <c r="B41" s="14"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="34"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="B42" s="15" t="s">
+      <c r="B42" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="C42" s="9" t="s">
+      <c r="C42" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="D42" s="15" t="s">
+      <c r="D42" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E42" s="18" t="s">
+      <c r="E42" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F42" s="6" t="s">
+      <c r="F42" s="25" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="13"/>
-      <c r="B43" s="16"/>
-      <c r="C43" s="10"/>
-      <c r="D43" s="16"/>
-      <c r="E43" s="19"/>
-      <c r="F43" s="7"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="13"/>
-      <c r="B44" s="16"/>
-      <c r="C44" s="10"/>
-      <c r="D44" s="16"/>
-      <c r="E44" s="19"/>
-      <c r="F44" s="7"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="14"/>
-      <c r="B45" s="17"/>
-      <c r="C45" s="11"/>
-      <c r="D45" s="17"/>
-      <c r="E45" s="20"/>
-      <c r="F45" s="8"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="12" t="s">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" s="10"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="22"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="26"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" s="10"/>
+      <c r="B44" s="13"/>
+      <c r="C44" s="22"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="16"/>
+      <c r="F44" s="26"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" s="11"/>
+      <c r="B45" s="14"/>
+      <c r="C45" s="23"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="17"/>
+      <c r="F45" s="27"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="B46" s="15" t="s">
+      <c r="B46" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="C46" s="9" t="s">
+      <c r="C46" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="D46" s="15" t="s">
+      <c r="D46" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E46" s="18" t="s">
+      <c r="E46" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F46" s="21" t="s">
+      <c r="F46" s="18" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="13"/>
-      <c r="B47" s="16"/>
-      <c r="C47" s="10"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="19"/>
-      <c r="F47" s="22"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="13"/>
-      <c r="B48" s="16"/>
-      <c r="C48" s="10"/>
-      <c r="D48" s="16"/>
-      <c r="E48" s="19"/>
-      <c r="F48" s="22"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="14"/>
-      <c r="B49" s="17"/>
-      <c r="C49" s="11"/>
-      <c r="D49" s="17"/>
-      <c r="E49" s="20"/>
-      <c r="F49" s="23"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="12" t="s">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" s="10"/>
+      <c r="B47" s="13"/>
+      <c r="C47" s="22"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="19"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" s="10"/>
+      <c r="B48" s="13"/>
+      <c r="C48" s="22"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="16"/>
+      <c r="F48" s="19"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" s="11"/>
+      <c r="B49" s="14"/>
+      <c r="C49" s="23"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="17"/>
+      <c r="F49" s="20"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="B50" s="15" t="s">
+      <c r="B50" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="C50" s="9" t="s">
+      <c r="C50" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="D50" s="15" t="s">
+      <c r="D50" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="E50" s="18" t="s">
+      <c r="E50" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F50" s="21" t="s">
+      <c r="F50" s="18" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="13"/>
-      <c r="B51" s="16"/>
-      <c r="C51" s="10"/>
-      <c r="D51" s="16"/>
-      <c r="E51" s="19"/>
-      <c r="F51" s="22"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="13"/>
-      <c r="B52" s="16"/>
-      <c r="C52" s="10"/>
-      <c r="D52" s="16"/>
-      <c r="E52" s="19"/>
-      <c r="F52" s="22"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="14"/>
-      <c r="B53" s="17"/>
-      <c r="C53" s="11"/>
-      <c r="D53" s="17"/>
-      <c r="E53" s="20"/>
-      <c r="F53" s="23"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="12" t="s">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" s="10"/>
+      <c r="B51" s="13"/>
+      <c r="C51" s="22"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="16"/>
+      <c r="F51" s="19"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" s="10"/>
+      <c r="B52" s="13"/>
+      <c r="C52" s="22"/>
+      <c r="D52" s="13"/>
+      <c r="E52" s="16"/>
+      <c r="F52" s="19"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" s="11"/>
+      <c r="B53" s="14"/>
+      <c r="C53" s="23"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="17"/>
+      <c r="F53" s="20"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="B54" s="15" t="s">
+      <c r="B54" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="C54" s="35" t="s">
+      <c r="C54" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="D54" s="15" t="s">
+      <c r="D54" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="E54" s="18" t="s">
+      <c r="E54" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F54" s="21" t="s">
+      <c r="F54" s="18" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="13"/>
-      <c r="B55" s="16"/>
-      <c r="C55" s="10"/>
-      <c r="D55" s="16"/>
-      <c r="E55" s="19"/>
-      <c r="F55" s="22"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="13"/>
-      <c r="B56" s="16"/>
-      <c r="C56" s="10"/>
-      <c r="D56" s="16"/>
-      <c r="E56" s="19"/>
-      <c r="F56" s="22"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="14"/>
-      <c r="B57" s="17"/>
-      <c r="C57" s="11"/>
-      <c r="D57" s="17"/>
-      <c r="E57" s="20"/>
-      <c r="F57" s="23"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="12" t="s">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" s="10"/>
+      <c r="B55" s="13"/>
+      <c r="C55" s="22"/>
+      <c r="D55" s="13"/>
+      <c r="E55" s="16"/>
+      <c r="F55" s="19"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" s="10"/>
+      <c r="B56" s="13"/>
+      <c r="C56" s="22"/>
+      <c r="D56" s="13"/>
+      <c r="E56" s="16"/>
+      <c r="F56" s="19"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" s="11"/>
+      <c r="B57" s="14"/>
+      <c r="C57" s="23"/>
+      <c r="D57" s="14"/>
+      <c r="E57" s="17"/>
+      <c r="F57" s="20"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="B58" s="15" t="s">
+      <c r="B58" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="C58" s="9" t="s">
+      <c r="C58" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="D58" s="15" t="s">
+      <c r="D58" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="E58" s="18" t="s">
+      <c r="E58" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F58" s="21" t="s">
+      <c r="F58" s="18" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="13"/>
-      <c r="B59" s="16"/>
-      <c r="C59" s="10"/>
-      <c r="D59" s="16"/>
-      <c r="E59" s="19"/>
-      <c r="F59" s="22"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="13"/>
-      <c r="B60" s="16"/>
-      <c r="C60" s="10"/>
-      <c r="D60" s="16"/>
-      <c r="E60" s="19"/>
-      <c r="F60" s="22"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="14"/>
-      <c r="B61" s="17"/>
-      <c r="C61" s="11"/>
-      <c r="D61" s="17"/>
-      <c r="E61" s="20"/>
-      <c r="F61" s="23"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="12" t="s">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" s="10"/>
+      <c r="B59" s="13"/>
+      <c r="C59" s="22"/>
+      <c r="D59" s="13"/>
+      <c r="E59" s="16"/>
+      <c r="F59" s="19"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" s="10"/>
+      <c r="B60" s="13"/>
+      <c r="C60" s="22"/>
+      <c r="D60" s="13"/>
+      <c r="E60" s="16"/>
+      <c r="F60" s="19"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" s="11"/>
+      <c r="B61" s="14"/>
+      <c r="C61" s="23"/>
+      <c r="D61" s="14"/>
+      <c r="E61" s="17"/>
+      <c r="F61" s="20"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="B62" s="15" t="s">
+      <c r="B62" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="C62" s="35" t="s">
+      <c r="C62" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="D62" s="15" t="s">
+      <c r="D62" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="E62" s="18" t="s">
+      <c r="E62" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F62" s="21" t="s">
+      <c r="F62" s="18" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="13"/>
-      <c r="B63" s="16"/>
-      <c r="C63" s="10"/>
-      <c r="D63" s="16"/>
-      <c r="E63" s="19"/>
-      <c r="F63" s="22"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="13"/>
-      <c r="B64" s="16"/>
-      <c r="C64" s="10"/>
-      <c r="D64" s="16"/>
-      <c r="E64" s="19"/>
-      <c r="F64" s="22"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="14"/>
-      <c r="B65" s="17"/>
-      <c r="C65" s="11"/>
-      <c r="D65" s="17"/>
-      <c r="E65" s="20"/>
-      <c r="F65" s="23"/>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="12" t="s">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" s="10"/>
+      <c r="B63" s="13"/>
+      <c r="C63" s="22"/>
+      <c r="D63" s="13"/>
+      <c r="E63" s="16"/>
+      <c r="F63" s="19"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" s="10"/>
+      <c r="B64" s="13"/>
+      <c r="C64" s="22"/>
+      <c r="D64" s="13"/>
+      <c r="E64" s="16"/>
+      <c r="F64" s="19"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65" s="11"/>
+      <c r="B65" s="14"/>
+      <c r="C65" s="23"/>
+      <c r="D65" s="14"/>
+      <c r="E65" s="17"/>
+      <c r="F65" s="20"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="B66" s="15" t="s">
+      <c r="B66" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="C66" s="35" t="s">
+      <c r="C66" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="D66" s="15" t="s">
+      <c r="D66" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E66" s="18" t="s">
+      <c r="E66" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F66" s="21" t="s">
+      <c r="F66" s="18" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="13"/>
-      <c r="B67" s="16"/>
-      <c r="C67" s="10"/>
-      <c r="D67" s="16"/>
-      <c r="E67" s="19"/>
-      <c r="F67" s="22"/>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="13"/>
-      <c r="B68" s="16"/>
-      <c r="C68" s="10"/>
-      <c r="D68" s="16"/>
-      <c r="E68" s="19"/>
-      <c r="F68" s="22"/>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="14"/>
-      <c r="B69" s="17"/>
-      <c r="C69" s="11"/>
-      <c r="D69" s="17"/>
-      <c r="E69" s="20"/>
-      <c r="F69" s="23"/>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="12" t="s">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A67" s="10"/>
+      <c r="B67" s="13"/>
+      <c r="C67" s="22"/>
+      <c r="D67" s="13"/>
+      <c r="E67" s="16"/>
+      <c r="F67" s="19"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A68" s="10"/>
+      <c r="B68" s="13"/>
+      <c r="C68" s="22"/>
+      <c r="D68" s="13"/>
+      <c r="E68" s="16"/>
+      <c r="F68" s="19"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A69" s="11"/>
+      <c r="B69" s="14"/>
+      <c r="C69" s="23"/>
+      <c r="D69" s="14"/>
+      <c r="E69" s="17"/>
+      <c r="F69" s="20"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A70" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B70" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C70" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="B70" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="C70" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="D70" s="15" t="s">
+      <c r="D70" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="E70" s="18" t="s">
+      <c r="E70" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F70" s="31" t="s">
+      <c r="F70" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="13"/>
-      <c r="B71" s="16"/>
-      <c r="C71" s="13"/>
-      <c r="D71" s="16"/>
-      <c r="E71" s="19"/>
-      <c r="F71" s="32"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="13"/>
-      <c r="B72" s="16"/>
-      <c r="C72" s="13"/>
-      <c r="D72" s="16"/>
-      <c r="E72" s="19"/>
-      <c r="F72" s="32"/>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="14"/>
-      <c r="B73" s="17"/>
-      <c r="C73" s="14"/>
-      <c r="D73" s="17"/>
-      <c r="E73" s="20"/>
-      <c r="F73" s="33"/>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A71" s="10"/>
+      <c r="B71" s="13"/>
+      <c r="C71" s="10"/>
+      <c r="D71" s="13"/>
+      <c r="E71" s="16"/>
+      <c r="F71" s="7"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A72" s="10"/>
+      <c r="B72" s="13"/>
+      <c r="C72" s="10"/>
+      <c r="D72" s="13"/>
+      <c r="E72" s="16"/>
+      <c r="F72" s="7"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A73" s="11"/>
+      <c r="B73" s="14"/>
+      <c r="C73" s="11"/>
+      <c r="D73" s="14"/>
+      <c r="E73" s="17"/>
+      <c r="F73" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="112">
-    <mergeCell ref="F70:F73"/>
-    <mergeCell ref="A70:A73"/>
-    <mergeCell ref="B70:B73"/>
-    <mergeCell ref="C70:C73"/>
-    <mergeCell ref="D70:D73"/>
-    <mergeCell ref="E70:E73"/>
-    <mergeCell ref="F62:F65"/>
-    <mergeCell ref="A66:A69"/>
-    <mergeCell ref="B66:B69"/>
-    <mergeCell ref="C66:C69"/>
-    <mergeCell ref="D66:D69"/>
-    <mergeCell ref="E66:E69"/>
-    <mergeCell ref="F66:F69"/>
-    <mergeCell ref="A62:A65"/>
-    <mergeCell ref="B62:B65"/>
-    <mergeCell ref="C62:C65"/>
-    <mergeCell ref="D62:D65"/>
-    <mergeCell ref="E62:E65"/>
+    <mergeCell ref="F42:F45"/>
+    <mergeCell ref="C42:C45"/>
+    <mergeCell ref="A46:A49"/>
+    <mergeCell ref="B46:B49"/>
+    <mergeCell ref="C46:C49"/>
+    <mergeCell ref="D46:D49"/>
+    <mergeCell ref="E46:E49"/>
+    <mergeCell ref="F46:F49"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="B42:B45"/>
+    <mergeCell ref="D42:D45"/>
+    <mergeCell ref="E42:E45"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="E30:E33"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="C26:C29"/>
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="E18:E21"/>
+    <mergeCell ref="E14:E17"/>
+    <mergeCell ref="F14:F17"/>
+    <mergeCell ref="D14:D17"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="F38:F41"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="D22:D25"/>
+    <mergeCell ref="F22:F25"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="F34:F37"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="F30:F33"/>
+    <mergeCell ref="E34:E37"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="F26:F29"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="E22:E25"/>
+    <mergeCell ref="E26:E29"/>
+    <mergeCell ref="E38:E41"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="D38:D41"/>
+    <mergeCell ref="C34:C37"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="F2:F5"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="F10:F13"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="F6:F9"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="E6:E9"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="F18:F21"/>
+    <mergeCell ref="C16:C17"/>
     <mergeCell ref="F58:F61"/>
     <mergeCell ref="H2:H5"/>
     <mergeCell ref="H6:H9"/>
@@ -2336,76 +2388,24 @@
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="D2:D5"/>
     <mergeCell ref="A38:A41"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="F2:F5"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="F10:F13"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="D6:D9"/>
-    <mergeCell ref="F6:F9"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="E2:E5"/>
-    <mergeCell ref="E6:E9"/>
-    <mergeCell ref="E10:E13"/>
-    <mergeCell ref="F38:F41"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="D22:D25"/>
-    <mergeCell ref="F22:F25"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="F34:F37"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="F30:F33"/>
-    <mergeCell ref="E34:E37"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="F26:F29"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="E22:E25"/>
-    <mergeCell ref="E26:E29"/>
-    <mergeCell ref="E38:E41"/>
-    <mergeCell ref="B38:B41"/>
-    <mergeCell ref="D38:D41"/>
-    <mergeCell ref="F18:F21"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="C34:C37"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="E30:E33"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="C26:C29"/>
-    <mergeCell ref="D18:D21"/>
-    <mergeCell ref="E18:E21"/>
-    <mergeCell ref="E14:E17"/>
-    <mergeCell ref="F14:F17"/>
-    <mergeCell ref="D14:D17"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="F42:F45"/>
-    <mergeCell ref="C42:C45"/>
-    <mergeCell ref="A46:A49"/>
-    <mergeCell ref="B46:B49"/>
-    <mergeCell ref="C46:C49"/>
-    <mergeCell ref="D46:D49"/>
-    <mergeCell ref="E46:E49"/>
-    <mergeCell ref="F46:F49"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="B42:B45"/>
-    <mergeCell ref="D42:D45"/>
-    <mergeCell ref="E42:E45"/>
+    <mergeCell ref="F70:F73"/>
+    <mergeCell ref="A70:A73"/>
+    <mergeCell ref="B70:B73"/>
+    <mergeCell ref="C70:C73"/>
+    <mergeCell ref="D70:D73"/>
+    <mergeCell ref="E70:E73"/>
+    <mergeCell ref="F62:F65"/>
+    <mergeCell ref="A66:A69"/>
+    <mergeCell ref="B66:B69"/>
+    <mergeCell ref="C66:C69"/>
+    <mergeCell ref="D66:D69"/>
+    <mergeCell ref="E66:E69"/>
+    <mergeCell ref="F66:F69"/>
+    <mergeCell ref="A62:A65"/>
+    <mergeCell ref="B62:B65"/>
+    <mergeCell ref="C62:C65"/>
+    <mergeCell ref="D62:D65"/>
+    <mergeCell ref="E62:E65"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
(EJECUTAR SCRIPT SQL) Diferenciacion Admin y Editor
Solo hay dos cosas que el admin puede hacer exclusivamente:
Vetar personas
Borrar reseñas ajenas
</commit_message>
<xml_diff>
--- a/ToDo/Product Backlog.xlsx
+++ b/ToDo/Product Backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juana\Escritorio\UNI\Tercero\Segundo Cuatrimestre\TaW\ArkhamMovies\ToDo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minie\Desktop\UMA\Tercer Curso\2do cuatrimestre\Tecnologías de Aplicaciones Web\Trabajo en grupo\ArkhamMovies\ToDo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4219A9AF-CCC9-493A-90B4-664F276F7EEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8603902A-1B82-4078-AAF0-C9CD17025354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{391AEB77-1329-4C84-A561-AE54ADC33E64}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{391AEB77-1329-4C84-A561-AE54ADC33E64}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -991,7 +991,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1006,6 +1006,63 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1015,53 +1072,8 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1081,28 +1093,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1441,20 +1432,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D14C92F-3F4B-401B-9B84-B21C184BF8CD}">
   <dimension ref="A1:H73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18:H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="34.109375" customWidth="1"/>
-    <col min="3" max="3" width="66.88671875" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" customWidth="1"/>
-    <col min="6" max="6" width="13.88671875" customWidth="1"/>
-    <col min="8" max="8" width="33.5546875" customWidth="1"/>
+    <col min="2" max="2" width="34.140625" customWidth="1"/>
+    <col min="3" max="3" width="66.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" customWidth="1"/>
+    <col min="8" max="8" width="33.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1477,877 +1468,922 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="H2" s="35" t="s">
+      <c r="H2" s="21" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="13"/>
-      <c r="B3" s="16"/>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="B3" s="13"/>
       <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="7"/>
-      <c r="H3" s="10"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="13"/>
-      <c r="B4" s="16"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="26"/>
+      <c r="H3" s="22"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="13"/>
       <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="7"/>
-      <c r="H4" s="10"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="14"/>
-      <c r="B5" s="17"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="26"/>
+      <c r="H4" s="22"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="8"/>
+      <c r="B5" s="14"/>
       <c r="C5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="17"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="8"/>
-      <c r="H5" s="11"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D5" s="14"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="27"/>
+      <c r="H5" s="23"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="25" t="s">
+      <c r="E6" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="H6" s="15" t="s">
+      <c r="H6" s="6" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="13"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="7"/>
-      <c r="H7" s="13"/>
-    </row>
-    <row r="8" spans="1:8" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="13"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="15" t="s">
+    <row r="7" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="26"/>
+      <c r="H7" s="7"/>
+    </row>
+    <row r="8" spans="1:8" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="7"/>
-      <c r="H8" s="13"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="14"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="8"/>
-      <c r="H9" s="14"/>
-    </row>
-    <row r="10" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D8" s="13"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="26"/>
+      <c r="H8" s="7"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="8"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="27"/>
+      <c r="H9" s="8"/>
+    </row>
+    <row r="10" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="25" t="s">
+      <c r="E10" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="25" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="13"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="7"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="13"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="15" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="26"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="16"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="7"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="14"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="8"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="26"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="27"/>
       <c r="H13" s="5" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="25" t="s">
+      <c r="E14" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="H14" s="36" t="s">
+      <c r="H14" s="6" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="13"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="7"/>
-      <c r="H15" s="37"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="13"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="9" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="26"/>
+      <c r="H15" s="7"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="7"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="16"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="7"/>
-      <c r="H16" s="37"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="14"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="8"/>
-      <c r="H17" s="38"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D16" s="13"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="26"/>
+      <c r="H16" s="7"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="27"/>
+      <c r="H17" s="8"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="E18" s="25" t="s">
+      <c r="E18" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="H18" s="36" t="s">
+      <c r="H18" s="21" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="13"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="7"/>
-      <c r="H19" s="37"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="13"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="9" t="s">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="7"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="26"/>
+      <c r="H19" s="22"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="7"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="16"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="7"/>
-      <c r="H20" s="37"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="14"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="8"/>
-      <c r="H21" s="38"/>
-    </row>
-    <row r="22" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D20" s="13"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="26"/>
+      <c r="H20" s="22"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="8"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="27"/>
+      <c r="H21" s="23"/>
+    </row>
+    <row r="22" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="6" t="s">
         <v>39</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D22" s="15" t="s">
+      <c r="D22" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E22" s="25" t="s">
+      <c r="E22" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="F22" s="21" t="s">
+      <c r="F22" s="18" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="13"/>
-      <c r="B23" s="16"/>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="7"/>
+      <c r="B23" s="13"/>
       <c r="C23" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="16"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="22"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="13"/>
-      <c r="B24" s="16"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="19"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="7"/>
+      <c r="B24" s="13"/>
       <c r="C24" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D24" s="16"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="22"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="14"/>
-      <c r="B25" s="17"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="19"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="8"/>
+      <c r="B25" s="14"/>
       <c r="C25" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="17"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="23"/>
-    </row>
-    <row r="26" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D25" s="14"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="20"/>
+    </row>
+    <row r="26" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="6" t="s">
         <v>32</v>
       </c>
       <c r="C26" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D26" s="15" t="s">
+      <c r="D26" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="E26" s="25" t="s">
+      <c r="E26" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="F26" s="31" t="s">
+      <c r="F26" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="13"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="32"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="13"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="32"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="14"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="33"/>
-    </row>
-    <row r="30" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="7"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="10"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="7"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="10"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="8"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="11"/>
+    </row>
+    <row r="30" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D30" s="15" t="s">
+      <c r="D30" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E30" s="18" t="s">
+      <c r="E30" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F30" s="31" t="s">
+      <c r="F30" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="13"/>
-      <c r="B31" s="16"/>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="7"/>
+      <c r="B31" s="13"/>
       <c r="C31" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D31" s="16"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="32"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="13"/>
-      <c r="B32" s="16"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="10"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="7"/>
+      <c r="B32" s="13"/>
       <c r="C32" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D32" s="16"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="32"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="14"/>
-      <c r="B33" s="17"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="10"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="8"/>
+      <c r="B33" s="14"/>
       <c r="C33" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D33" s="17"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="33"/>
-    </row>
-    <row r="34" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D33" s="14"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="11"/>
+    </row>
+    <row r="34" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="B34" s="15" t="s">
+      <c r="B34" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="9" t="s">
+      <c r="C34" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="D34" s="15" t="s">
+      <c r="D34" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="E34" s="18" t="s">
+      <c r="E34" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F34" s="31" t="s">
+      <c r="F34" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="13"/>
-      <c r="B35" s="16"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="32"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="13"/>
-      <c r="B36" s="16"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="19"/>
-      <c r="F36" s="32"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="14"/>
-      <c r="B37" s="17"/>
-      <c r="C37" s="11"/>
-      <c r="D37" s="17"/>
-      <c r="E37" s="20"/>
-      <c r="F37" s="33"/>
-    </row>
-    <row r="38" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="7"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="10"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="7"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="10"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="8"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="23"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="11"/>
+    </row>
+    <row r="38" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="B38" s="15" t="s">
+      <c r="B38" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C38" s="9" t="s">
+      <c r="C38" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="D38" s="15" t="s">
+      <c r="D38" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E38" s="18" t="s">
+      <c r="E38" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F38" s="28" t="s">
+      <c r="F38" s="32" t="s">
         <v>57</v>
       </c>
       <c r="G38" s="4"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="13"/>
-      <c r="B39" s="16"/>
-      <c r="C39" s="11"/>
-      <c r="D39" s="16"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="29"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="13"/>
-      <c r="B40" s="16"/>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="7"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="23"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="33"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="7"/>
+      <c r="B40" s="13"/>
       <c r="C40" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D40" s="16"/>
-      <c r="E40" s="19"/>
-      <c r="F40" s="29"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="14"/>
-      <c r="B41" s="17"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="17"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="30"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D40" s="13"/>
+      <c r="E40" s="16"/>
+      <c r="F40" s="33"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="8"/>
+      <c r="B41" s="14"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="34"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="B42" s="15" t="s">
+      <c r="B42" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="C42" s="9" t="s">
+      <c r="C42" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="D42" s="15" t="s">
+      <c r="D42" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E42" s="18" t="s">
+      <c r="E42" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F42" s="6" t="s">
+      <c r="F42" s="25" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="13"/>
-      <c r="B43" s="16"/>
-      <c r="C43" s="10"/>
-      <c r="D43" s="16"/>
-      <c r="E43" s="19"/>
-      <c r="F43" s="7"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="13"/>
-      <c r="B44" s="16"/>
-      <c r="C44" s="10"/>
-      <c r="D44" s="16"/>
-      <c r="E44" s="19"/>
-      <c r="F44" s="7"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="14"/>
-      <c r="B45" s="17"/>
-      <c r="C45" s="11"/>
-      <c r="D45" s="17"/>
-      <c r="E45" s="20"/>
-      <c r="F45" s="8"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="7"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="22"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="26"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="7"/>
+      <c r="B44" s="13"/>
+      <c r="C44" s="22"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="16"/>
+      <c r="F44" s="26"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="8"/>
+      <c r="B45" s="14"/>
+      <c r="C45" s="23"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="17"/>
+      <c r="F45" s="27"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="B46" s="15" t="s">
+      <c r="B46" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C46" s="9" t="s">
+      <c r="C46" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="D46" s="15" t="s">
+      <c r="D46" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E46" s="18" t="s">
+      <c r="E46" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F46" s="21" t="s">
+      <c r="F46" s="18" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="13"/>
-      <c r="B47" s="16"/>
-      <c r="C47" s="10"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="19"/>
-      <c r="F47" s="22"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="13"/>
-      <c r="B48" s="16"/>
-      <c r="C48" s="10"/>
-      <c r="D48" s="16"/>
-      <c r="E48" s="19"/>
-      <c r="F48" s="22"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" s="14"/>
-      <c r="B49" s="17"/>
-      <c r="C49" s="11"/>
-      <c r="D49" s="17"/>
-      <c r="E49" s="20"/>
-      <c r="F49" s="23"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="7"/>
+      <c r="B47" s="13"/>
+      <c r="C47" s="22"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="19"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="7"/>
+      <c r="B48" s="13"/>
+      <c r="C48" s="22"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="16"/>
+      <c r="F48" s="19"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="8"/>
+      <c r="B49" s="14"/>
+      <c r="C49" s="23"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="17"/>
+      <c r="F49" s="20"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="B50" s="15" t="s">
+      <c r="B50" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="C50" s="9" t="s">
+      <c r="C50" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="D50" s="15" t="s">
+      <c r="D50" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="E50" s="18" t="s">
+      <c r="E50" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F50" s="21" t="s">
+      <c r="F50" s="18" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="13"/>
-      <c r="B51" s="16"/>
-      <c r="C51" s="10"/>
-      <c r="D51" s="16"/>
-      <c r="E51" s="19"/>
-      <c r="F51" s="22"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" s="13"/>
-      <c r="B52" s="16"/>
-      <c r="C52" s="10"/>
-      <c r="D52" s="16"/>
-      <c r="E52" s="19"/>
-      <c r="F52" s="22"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" s="14"/>
-      <c r="B53" s="17"/>
-      <c r="C53" s="11"/>
-      <c r="D53" s="17"/>
-      <c r="E53" s="20"/>
-      <c r="F53" s="23"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="7"/>
+      <c r="B51" s="13"/>
+      <c r="C51" s="22"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="16"/>
+      <c r="F51" s="19"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="7"/>
+      <c r="B52" s="13"/>
+      <c r="C52" s="22"/>
+      <c r="D52" s="13"/>
+      <c r="E52" s="16"/>
+      <c r="F52" s="19"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="8"/>
+      <c r="B53" s="14"/>
+      <c r="C53" s="23"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="17"/>
+      <c r="F53" s="20"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="B54" s="15" t="s">
+      <c r="B54" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="C54" s="35" t="s">
+      <c r="C54" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="D54" s="15" t="s">
+      <c r="D54" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="E54" s="18" t="s">
+      <c r="E54" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F54" s="21" t="s">
+      <c r="F54" s="18" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" s="13"/>
-      <c r="B55" s="16"/>
-      <c r="C55" s="10"/>
-      <c r="D55" s="16"/>
-      <c r="E55" s="19"/>
-      <c r="F55" s="22"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" s="13"/>
-      <c r="B56" s="16"/>
-      <c r="C56" s="10"/>
-      <c r="D56" s="16"/>
-      <c r="E56" s="19"/>
-      <c r="F56" s="22"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A57" s="14"/>
-      <c r="B57" s="17"/>
-      <c r="C57" s="11"/>
-      <c r="D57" s="17"/>
-      <c r="E57" s="20"/>
-      <c r="F57" s="23"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="7"/>
+      <c r="B55" s="13"/>
+      <c r="C55" s="22"/>
+      <c r="D55" s="13"/>
+      <c r="E55" s="16"/>
+      <c r="F55" s="19"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="7"/>
+      <c r="B56" s="13"/>
+      <c r="C56" s="22"/>
+      <c r="D56" s="13"/>
+      <c r="E56" s="16"/>
+      <c r="F56" s="19"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="8"/>
+      <c r="B57" s="14"/>
+      <c r="C57" s="23"/>
+      <c r="D57" s="14"/>
+      <c r="E57" s="17"/>
+      <c r="F57" s="20"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="B58" s="15" t="s">
+      <c r="B58" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="C58" s="9" t="s">
+      <c r="C58" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="D58" s="15" t="s">
+      <c r="D58" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="E58" s="18" t="s">
+      <c r="E58" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F58" s="21" t="s">
+      <c r="F58" s="18" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" s="13"/>
-      <c r="B59" s="16"/>
-      <c r="C59" s="10"/>
-      <c r="D59" s="16"/>
-      <c r="E59" s="19"/>
-      <c r="F59" s="22"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A60" s="13"/>
-      <c r="B60" s="16"/>
-      <c r="C60" s="10"/>
-      <c r="D60" s="16"/>
-      <c r="E60" s="19"/>
-      <c r="F60" s="22"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A61" s="14"/>
-      <c r="B61" s="17"/>
-      <c r="C61" s="11"/>
-      <c r="D61" s="17"/>
-      <c r="E61" s="20"/>
-      <c r="F61" s="23"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="7"/>
+      <c r="B59" s="13"/>
+      <c r="C59" s="22"/>
+      <c r="D59" s="13"/>
+      <c r="E59" s="16"/>
+      <c r="F59" s="19"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="7"/>
+      <c r="B60" s="13"/>
+      <c r="C60" s="22"/>
+      <c r="D60" s="13"/>
+      <c r="E60" s="16"/>
+      <c r="F60" s="19"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="8"/>
+      <c r="B61" s="14"/>
+      <c r="C61" s="23"/>
+      <c r="D61" s="14"/>
+      <c r="E61" s="17"/>
+      <c r="F61" s="20"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="B62" s="15" t="s">
+      <c r="B62" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="C62" s="35" t="s">
+      <c r="C62" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="D62" s="15" t="s">
+      <c r="D62" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="E62" s="18" t="s">
+      <c r="E62" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F62" s="21" t="s">
+      <c r="F62" s="18" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A63" s="13"/>
-      <c r="B63" s="16"/>
-      <c r="C63" s="10"/>
-      <c r="D63" s="16"/>
-      <c r="E63" s="19"/>
-      <c r="F63" s="22"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A64" s="13"/>
-      <c r="B64" s="16"/>
-      <c r="C64" s="10"/>
-      <c r="D64" s="16"/>
-      <c r="E64" s="19"/>
-      <c r="F64" s="22"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A65" s="14"/>
-      <c r="B65" s="17"/>
-      <c r="C65" s="11"/>
-      <c r="D65" s="17"/>
-      <c r="E65" s="20"/>
-      <c r="F65" s="23"/>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="7"/>
+      <c r="B63" s="13"/>
+      <c r="C63" s="22"/>
+      <c r="D63" s="13"/>
+      <c r="E63" s="16"/>
+      <c r="F63" s="19"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="7"/>
+      <c r="B64" s="13"/>
+      <c r="C64" s="22"/>
+      <c r="D64" s="13"/>
+      <c r="E64" s="16"/>
+      <c r="F64" s="19"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="8"/>
+      <c r="B65" s="14"/>
+      <c r="C65" s="23"/>
+      <c r="D65" s="14"/>
+      <c r="E65" s="17"/>
+      <c r="F65" s="20"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B66" s="15" t="s">
+      <c r="B66" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="C66" s="35" t="s">
+      <c r="C66" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="D66" s="15" t="s">
+      <c r="D66" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E66" s="18" t="s">
+      <c r="E66" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F66" s="21" t="s">
+      <c r="F66" s="18" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A67" s="13"/>
-      <c r="B67" s="16"/>
-      <c r="C67" s="10"/>
-      <c r="D67" s="16"/>
-      <c r="E67" s="19"/>
-      <c r="F67" s="22"/>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A68" s="13"/>
-      <c r="B68" s="16"/>
-      <c r="C68" s="10"/>
-      <c r="D68" s="16"/>
-      <c r="E68" s="19"/>
-      <c r="F68" s="22"/>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A69" s="14"/>
-      <c r="B69" s="17"/>
-      <c r="C69" s="11"/>
-      <c r="D69" s="17"/>
-      <c r="E69" s="20"/>
-      <c r="F69" s="23"/>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="7"/>
+      <c r="B67" s="13"/>
+      <c r="C67" s="22"/>
+      <c r="D67" s="13"/>
+      <c r="E67" s="16"/>
+      <c r="F67" s="19"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="7"/>
+      <c r="B68" s="13"/>
+      <c r="C68" s="22"/>
+      <c r="D68" s="13"/>
+      <c r="E68" s="16"/>
+      <c r="F68" s="19"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="8"/>
+      <c r="B69" s="14"/>
+      <c r="C69" s="23"/>
+      <c r="D69" s="14"/>
+      <c r="E69" s="17"/>
+      <c r="F69" s="20"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="B70" s="15" t="s">
+      <c r="B70" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C70" s="15" t="s">
+      <c r="C70" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="D70" s="15" t="s">
+      <c r="D70" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="E70" s="18" t="s">
+      <c r="E70" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F70" s="31" t="s">
+      <c r="F70" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A71" s="13"/>
-      <c r="B71" s="16"/>
-      <c r="C71" s="13"/>
-      <c r="D71" s="16"/>
-      <c r="E71" s="19"/>
-      <c r="F71" s="32"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A72" s="13"/>
-      <c r="B72" s="16"/>
-      <c r="C72" s="13"/>
-      <c r="D72" s="16"/>
-      <c r="E72" s="19"/>
-      <c r="F72" s="32"/>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A73" s="14"/>
-      <c r="B73" s="17"/>
-      <c r="C73" s="14"/>
-      <c r="D73" s="17"/>
-      <c r="E73" s="20"/>
-      <c r="F73" s="33"/>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="7"/>
+      <c r="B71" s="13"/>
+      <c r="C71" s="7"/>
+      <c r="D71" s="13"/>
+      <c r="E71" s="16"/>
+      <c r="F71" s="10"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="7"/>
+      <c r="B72" s="13"/>
+      <c r="C72" s="7"/>
+      <c r="D72" s="13"/>
+      <c r="E72" s="16"/>
+      <c r="F72" s="10"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="8"/>
+      <c r="B73" s="14"/>
+      <c r="C73" s="8"/>
+      <c r="D73" s="14"/>
+      <c r="E73" s="17"/>
+      <c r="F73" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="114">
-    <mergeCell ref="H14:H17"/>
-    <mergeCell ref="H18:H21"/>
-    <mergeCell ref="F70:F73"/>
-    <mergeCell ref="A70:A73"/>
-    <mergeCell ref="B70:B73"/>
-    <mergeCell ref="C70:C73"/>
-    <mergeCell ref="D70:D73"/>
-    <mergeCell ref="E70:E73"/>
-    <mergeCell ref="F62:F65"/>
-    <mergeCell ref="A66:A69"/>
-    <mergeCell ref="B66:B69"/>
-    <mergeCell ref="C66:C69"/>
-    <mergeCell ref="D66:D69"/>
-    <mergeCell ref="E66:E69"/>
-    <mergeCell ref="F66:F69"/>
-    <mergeCell ref="A62:A65"/>
-    <mergeCell ref="B62:B65"/>
-    <mergeCell ref="C62:C65"/>
-    <mergeCell ref="D62:D65"/>
-    <mergeCell ref="E62:E65"/>
-    <mergeCell ref="F58:F61"/>
+    <mergeCell ref="F42:F45"/>
+    <mergeCell ref="C42:C45"/>
+    <mergeCell ref="A46:A49"/>
+    <mergeCell ref="B46:B49"/>
+    <mergeCell ref="C46:C49"/>
+    <mergeCell ref="D46:D49"/>
+    <mergeCell ref="E46:E49"/>
+    <mergeCell ref="F46:F49"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="B42:B45"/>
+    <mergeCell ref="D42:D45"/>
+    <mergeCell ref="E42:E45"/>
+    <mergeCell ref="E30:E33"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="C26:C29"/>
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="E18:E21"/>
+    <mergeCell ref="E14:E17"/>
+    <mergeCell ref="F14:F17"/>
+    <mergeCell ref="D14:D17"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="F38:F41"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="D22:D25"/>
+    <mergeCell ref="F22:F25"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="F34:F37"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="F30:F33"/>
+    <mergeCell ref="E34:E37"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="F26:F29"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="E22:E25"/>
+    <mergeCell ref="E26:E29"/>
+    <mergeCell ref="E38:E41"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="D38:D41"/>
+    <mergeCell ref="C34:C37"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="F2:F5"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="F10:F13"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="F6:F9"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="E6:E9"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="F18:F21"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="C18:C19"/>
     <mergeCell ref="H2:H5"/>
     <mergeCell ref="H6:H9"/>
     <mergeCell ref="A58:A61"/>
@@ -2372,75 +2408,30 @@
     <mergeCell ref="D2:D5"/>
     <mergeCell ref="A38:A41"/>
     <mergeCell ref="A14:A17"/>
+    <mergeCell ref="H14:H17"/>
+    <mergeCell ref="H18:H21"/>
+    <mergeCell ref="F70:F73"/>
+    <mergeCell ref="A70:A73"/>
+    <mergeCell ref="B70:B73"/>
+    <mergeCell ref="C70:C73"/>
+    <mergeCell ref="D70:D73"/>
+    <mergeCell ref="E70:E73"/>
+    <mergeCell ref="F62:F65"/>
+    <mergeCell ref="A66:A69"/>
+    <mergeCell ref="B66:B69"/>
+    <mergeCell ref="C66:C69"/>
+    <mergeCell ref="D66:D69"/>
+    <mergeCell ref="E66:E69"/>
+    <mergeCell ref="F66:F69"/>
+    <mergeCell ref="A62:A65"/>
+    <mergeCell ref="B62:B65"/>
+    <mergeCell ref="C62:C65"/>
+    <mergeCell ref="D62:D65"/>
+    <mergeCell ref="E62:E65"/>
+    <mergeCell ref="F58:F61"/>
     <mergeCell ref="B26:B29"/>
     <mergeCell ref="A26:A29"/>
     <mergeCell ref="B14:B17"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="F2:F5"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="F10:F13"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="D6:D9"/>
-    <mergeCell ref="F6:F9"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="E2:E5"/>
-    <mergeCell ref="E6:E9"/>
-    <mergeCell ref="E10:E13"/>
-    <mergeCell ref="F18:F21"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="F38:F41"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="D22:D25"/>
-    <mergeCell ref="F22:F25"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="F34:F37"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="F30:F33"/>
-    <mergeCell ref="E34:E37"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="F26:F29"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="E22:E25"/>
-    <mergeCell ref="E26:E29"/>
-    <mergeCell ref="E38:E41"/>
-    <mergeCell ref="B38:B41"/>
-    <mergeCell ref="D38:D41"/>
-    <mergeCell ref="C34:C37"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="E30:E33"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="C26:C29"/>
-    <mergeCell ref="D18:D21"/>
-    <mergeCell ref="E18:E21"/>
-    <mergeCell ref="E14:E17"/>
-    <mergeCell ref="F14:F17"/>
-    <mergeCell ref="D14:D17"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="F42:F45"/>
-    <mergeCell ref="C42:C45"/>
-    <mergeCell ref="A46:A49"/>
-    <mergeCell ref="B46:B49"/>
-    <mergeCell ref="C46:C49"/>
-    <mergeCell ref="D46:D49"/>
-    <mergeCell ref="E46:E49"/>
-    <mergeCell ref="F46:F49"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="B42:B45"/>
-    <mergeCell ref="D42:D45"/>
-    <mergeCell ref="E42:E45"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Crear y Editar película con todos los parámetros
</commit_message>
<xml_diff>
--- a/ToDo/Product Backlog.xlsx
+++ b/ToDo/Product Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minie\Desktop\UMA\Tercer Curso\2do cuatrimestre\Tecnologías de Aplicaciones Web\Trabajo en grupo\ArkhamMovies\ToDo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8603902A-1B82-4078-AAF0-C9CD17025354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{546CCD43-244B-40A0-B9AD-C5EA1F3DC3F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{391AEB77-1329-4C84-A561-AE54ADC33E64}"/>
   </bookViews>
@@ -1006,14 +1006,80 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1024,77 +1090,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1432,8 +1432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D14C92F-3F4B-401B-9B84-B21C184BF8CD}">
   <dimension ref="A1:H73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18:H21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E76" sqref="E76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1472,155 +1472,155 @@
       <c r="A2" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="15" t="s">
         <v>25</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="35" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="13"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="16"/>
       <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="26"/>
-      <c r="H3" s="22"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="7"/>
+      <c r="H3" s="10"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="13"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="26"/>
-      <c r="H4" s="22"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="7"/>
+      <c r="H4" s="10"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="14"/>
+      <c r="A5" s="14"/>
+      <c r="B5" s="17"/>
       <c r="C5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="27"/>
-      <c r="H5" s="23"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="8"/>
+      <c r="H5" s="11"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="29" t="s">
+      <c r="E6" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="25" t="s">
+      <c r="F6" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="15" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="26"/>
-      <c r="H7" s="7"/>
+      <c r="A7" s="13"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="7"/>
+      <c r="H7" s="13"/>
     </row>
     <row r="8" spans="1:8" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="6" t="s">
+      <c r="A8" s="13"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="26"/>
-      <c r="H8" s="7"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="7"/>
+      <c r="H8" s="13"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="27"/>
-      <c r="H9" s="8"/>
+      <c r="A9" s="14"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="8"/>
+      <c r="H9" s="14"/>
     </row>
     <row r="10" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="29" t="s">
+      <c r="E10" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="25" t="s">
+      <c r="F10" s="6" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="26"/>
+      <c r="A11" s="13"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="7"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="6" t="s">
+      <c r="A12" s="13"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="26"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="7"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="27"/>
+      <c r="A13" s="14"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="8"/>
       <c r="H13" s="5" t="s">
         <v>86</v>
       </c>
@@ -1629,716 +1629,764 @@
       <c r="A14" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="24" t="s">
+      <c r="C14" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="29" t="s">
+      <c r="E14" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="25" t="s">
+      <c r="F14" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="H14" s="6" t="s">
+      <c r="H14" s="35" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="26"/>
-      <c r="H15" s="7"/>
+      <c r="A15" s="13"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="7"/>
+      <c r="H15" s="10"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="24" t="s">
+      <c r="A16" s="13"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="13"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="26"/>
-      <c r="H16" s="7"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="7"/>
+      <c r="H16" s="10"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="27"/>
-      <c r="H17" s="8"/>
+      <c r="A17" s="14"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="8"/>
+      <c r="H17" s="11"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="24" t="s">
+      <c r="C18" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="E18" s="29" t="s">
+      <c r="E18" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="F18" s="25" t="s">
+      <c r="F18" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="H18" s="21" t="s">
+      <c r="H18" s="35" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="26"/>
-      <c r="H19" s="22"/>
+      <c r="A19" s="13"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="7"/>
+      <c r="H19" s="10"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="24" t="s">
+      <c r="A20" s="13"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="13"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="26"/>
-      <c r="H20" s="22"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="7"/>
+      <c r="H20" s="10"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="35"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="27"/>
-      <c r="H21" s="23"/>
+      <c r="A21" s="14"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="8"/>
+      <c r="H21" s="11"/>
     </row>
     <row r="22" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="15" t="s">
         <v>39</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="E22" s="29" t="s">
+      <c r="E22" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="F22" s="18" t="s">
+      <c r="F22" s="21" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
-      <c r="B23" s="13"/>
+      <c r="A23" s="13"/>
+      <c r="B23" s="16"/>
       <c r="C23" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="13"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="19"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="22"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24" s="13"/>
+      <c r="A24" s="13"/>
+      <c r="B24" s="16"/>
       <c r="C24" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D24" s="13"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="19"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="22"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="14"/>
+      <c r="A25" s="14"/>
+      <c r="B25" s="17"/>
       <c r="C25" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="14"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="20"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="23"/>
     </row>
     <row r="26" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="15" t="s">
         <v>32</v>
       </c>
       <c r="C26" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D26" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="E26" s="29" t="s">
+      <c r="E26" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="F26" s="9" t="s">
+      <c r="F26" s="31" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
-      <c r="B27" s="13"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="10"/>
+      <c r="A27" s="13"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="32"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="10"/>
+      <c r="A28" s="13"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="32"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="8"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="11"/>
+      <c r="A29" s="14"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="33"/>
     </row>
     <row r="30" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="15" t="s">
         <v>15</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D30" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E30" s="15" t="s">
+      <c r="E30" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F30" s="9" t="s">
+      <c r="F30" s="31" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
-      <c r="B31" s="13"/>
+      <c r="A31" s="13"/>
+      <c r="B31" s="16"/>
       <c r="C31" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D31" s="13"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="10"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="32"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
-      <c r="B32" s="13"/>
+      <c r="A32" s="13"/>
+      <c r="B32" s="16"/>
       <c r="C32" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D32" s="13"/>
-      <c r="E32" s="16"/>
-      <c r="F32" s="10"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="32"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="8"/>
-      <c r="B33" s="14"/>
+      <c r="A33" s="14"/>
+      <c r="B33" s="17"/>
       <c r="C33" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D33" s="14"/>
-      <c r="E33" s="17"/>
-      <c r="F33" s="11"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="33"/>
     </row>
     <row r="34" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="24" t="s">
+      <c r="C34" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="D34" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="E34" s="15" t="s">
+      <c r="E34" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F34" s="9" t="s">
+      <c r="F34" s="31" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="7"/>
-      <c r="B35" s="13"/>
-      <c r="C35" s="22"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="10"/>
+      <c r="A35" s="13"/>
+      <c r="B35" s="16"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="32"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="7"/>
-      <c r="B36" s="13"/>
-      <c r="C36" s="22"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="16"/>
-      <c r="F36" s="10"/>
+      <c r="A36" s="13"/>
+      <c r="B36" s="16"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="32"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="8"/>
-      <c r="B37" s="14"/>
-      <c r="C37" s="23"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="17"/>
-      <c r="F37" s="11"/>
+      <c r="A37" s="14"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="33"/>
     </row>
     <row r="38" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C38" s="24" t="s">
+      <c r="C38" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D38" s="6" t="s">
+      <c r="D38" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="E38" s="15" t="s">
+      <c r="E38" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F38" s="32" t="s">
+      <c r="F38" s="28" t="s">
         <v>57</v>
       </c>
       <c r="G38" s="4"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="7"/>
-      <c r="B39" s="13"/>
-      <c r="C39" s="23"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="16"/>
-      <c r="F39" s="33"/>
+      <c r="A39" s="13"/>
+      <c r="B39" s="16"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="29"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="7"/>
-      <c r="B40" s="13"/>
+      <c r="A40" s="13"/>
+      <c r="B40" s="16"/>
       <c r="C40" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D40" s="13"/>
-      <c r="E40" s="16"/>
-      <c r="F40" s="33"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="29"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="8"/>
-      <c r="B41" s="14"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="17"/>
-      <c r="F41" s="34"/>
+      <c r="A41" s="14"/>
+      <c r="B41" s="17"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="30"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="C42" s="24" t="s">
+      <c r="C42" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D42" s="6" t="s">
+      <c r="D42" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="E42" s="15" t="s">
+      <c r="E42" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F42" s="25" t="s">
+      <c r="F42" s="6" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="7"/>
-      <c r="B43" s="13"/>
-      <c r="C43" s="22"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="16"/>
-      <c r="F43" s="26"/>
+      <c r="A43" s="13"/>
+      <c r="B43" s="16"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="7"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="7"/>
-      <c r="B44" s="13"/>
-      <c r="C44" s="22"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="16"/>
-      <c r="F44" s="26"/>
+      <c r="A44" s="13"/>
+      <c r="B44" s="16"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="16"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="7"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="8"/>
-      <c r="B45" s="14"/>
-      <c r="C45" s="23"/>
-      <c r="D45" s="14"/>
-      <c r="E45" s="17"/>
-      <c r="F45" s="27"/>
+      <c r="A45" s="14"/>
+      <c r="B45" s="17"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="17"/>
+      <c r="E45" s="20"/>
+      <c r="F45" s="8"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="B46" s="6" t="s">
+      <c r="B46" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="C46" s="24" t="s">
+      <c r="C46" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="D46" s="6" t="s">
+      <c r="D46" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="E46" s="15" t="s">
+      <c r="E46" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F46" s="18" t="s">
+      <c r="F46" s="21" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="7"/>
-      <c r="B47" s="13"/>
-      <c r="C47" s="22"/>
-      <c r="D47" s="13"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="19"/>
+      <c r="A47" s="13"/>
+      <c r="B47" s="16"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="19"/>
+      <c r="F47" s="22"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="7"/>
-      <c r="B48" s="13"/>
-      <c r="C48" s="22"/>
-      <c r="D48" s="13"/>
-      <c r="E48" s="16"/>
-      <c r="F48" s="19"/>
+      <c r="A48" s="13"/>
+      <c r="B48" s="16"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="16"/>
+      <c r="E48" s="19"/>
+      <c r="F48" s="22"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="8"/>
-      <c r="B49" s="14"/>
-      <c r="C49" s="23"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="17"/>
-      <c r="F49" s="20"/>
+      <c r="A49" s="14"/>
+      <c r="B49" s="17"/>
+      <c r="C49" s="11"/>
+      <c r="D49" s="17"/>
+      <c r="E49" s="20"/>
+      <c r="F49" s="23"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="B50" s="6" t="s">
+      <c r="B50" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="C50" s="24" t="s">
+      <c r="C50" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D50" s="6" t="s">
+      <c r="D50" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="E50" s="15" t="s">
+      <c r="E50" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F50" s="18" t="s">
+      <c r="F50" s="21" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="7"/>
-      <c r="B51" s="13"/>
-      <c r="C51" s="22"/>
-      <c r="D51" s="13"/>
-      <c r="E51" s="16"/>
-      <c r="F51" s="19"/>
+      <c r="A51" s="13"/>
+      <c r="B51" s="16"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="16"/>
+      <c r="E51" s="19"/>
+      <c r="F51" s="22"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="7"/>
-      <c r="B52" s="13"/>
-      <c r="C52" s="22"/>
-      <c r="D52" s="13"/>
-      <c r="E52" s="16"/>
-      <c r="F52" s="19"/>
+      <c r="A52" s="13"/>
+      <c r="B52" s="16"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="16"/>
+      <c r="E52" s="19"/>
+      <c r="F52" s="22"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="8"/>
-      <c r="B53" s="14"/>
-      <c r="C53" s="23"/>
-      <c r="D53" s="14"/>
-      <c r="E53" s="17"/>
-      <c r="F53" s="20"/>
+      <c r="A53" s="14"/>
+      <c r="B53" s="17"/>
+      <c r="C53" s="11"/>
+      <c r="D53" s="17"/>
+      <c r="E53" s="20"/>
+      <c r="F53" s="23"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="B54" s="6" t="s">
+      <c r="B54" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="C54" s="21" t="s">
+      <c r="C54" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="D54" s="6" t="s">
+      <c r="D54" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="E54" s="15" t="s">
+      <c r="E54" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F54" s="18" t="s">
+      <c r="F54" s="21" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="7"/>
-      <c r="B55" s="13"/>
-      <c r="C55" s="22"/>
-      <c r="D55" s="13"/>
-      <c r="E55" s="16"/>
-      <c r="F55" s="19"/>
+      <c r="A55" s="13"/>
+      <c r="B55" s="16"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="16"/>
+      <c r="E55" s="19"/>
+      <c r="F55" s="22"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="7"/>
-      <c r="B56" s="13"/>
-      <c r="C56" s="22"/>
-      <c r="D56" s="13"/>
-      <c r="E56" s="16"/>
-      <c r="F56" s="19"/>
+      <c r="A56" s="13"/>
+      <c r="B56" s="16"/>
+      <c r="C56" s="10"/>
+      <c r="D56" s="16"/>
+      <c r="E56" s="19"/>
+      <c r="F56" s="22"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="8"/>
-      <c r="B57" s="14"/>
-      <c r="C57" s="23"/>
-      <c r="D57" s="14"/>
-      <c r="E57" s="17"/>
-      <c r="F57" s="20"/>
+      <c r="A57" s="14"/>
+      <c r="B57" s="17"/>
+      <c r="C57" s="11"/>
+      <c r="D57" s="17"/>
+      <c r="E57" s="20"/>
+      <c r="F57" s="23"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="B58" s="6" t="s">
+      <c r="B58" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="C58" s="24" t="s">
+      <c r="C58" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="D58" s="6" t="s">
+      <c r="D58" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="E58" s="15" t="s">
+      <c r="E58" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F58" s="18" t="s">
+      <c r="F58" s="21" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="7"/>
-      <c r="B59" s="13"/>
-      <c r="C59" s="22"/>
-      <c r="D59" s="13"/>
-      <c r="E59" s="16"/>
-      <c r="F59" s="19"/>
+      <c r="A59" s="13"/>
+      <c r="B59" s="16"/>
+      <c r="C59" s="10"/>
+      <c r="D59" s="16"/>
+      <c r="E59" s="19"/>
+      <c r="F59" s="22"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="7"/>
-      <c r="B60" s="13"/>
-      <c r="C60" s="22"/>
-      <c r="D60" s="13"/>
-      <c r="E60" s="16"/>
-      <c r="F60" s="19"/>
+      <c r="A60" s="13"/>
+      <c r="B60" s="16"/>
+      <c r="C60" s="10"/>
+      <c r="D60" s="16"/>
+      <c r="E60" s="19"/>
+      <c r="F60" s="22"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="8"/>
-      <c r="B61" s="14"/>
-      <c r="C61" s="23"/>
-      <c r="D61" s="14"/>
-      <c r="E61" s="17"/>
-      <c r="F61" s="20"/>
+      <c r="A61" s="14"/>
+      <c r="B61" s="17"/>
+      <c r="C61" s="11"/>
+      <c r="D61" s="17"/>
+      <c r="E61" s="20"/>
+      <c r="F61" s="23"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="B62" s="6" t="s">
+      <c r="B62" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="C62" s="21" t="s">
+      <c r="C62" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="D62" s="6" t="s">
+      <c r="D62" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="E62" s="15" t="s">
+      <c r="E62" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F62" s="18" t="s">
+      <c r="F62" s="21" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="7"/>
-      <c r="B63" s="13"/>
-      <c r="C63" s="22"/>
-      <c r="D63" s="13"/>
-      <c r="E63" s="16"/>
-      <c r="F63" s="19"/>
+      <c r="A63" s="13"/>
+      <c r="B63" s="16"/>
+      <c r="C63" s="10"/>
+      <c r="D63" s="16"/>
+      <c r="E63" s="19"/>
+      <c r="F63" s="22"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="7"/>
-      <c r="B64" s="13"/>
-      <c r="C64" s="22"/>
-      <c r="D64" s="13"/>
-      <c r="E64" s="16"/>
-      <c r="F64" s="19"/>
+      <c r="A64" s="13"/>
+      <c r="B64" s="16"/>
+      <c r="C64" s="10"/>
+      <c r="D64" s="16"/>
+      <c r="E64" s="19"/>
+      <c r="F64" s="22"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="8"/>
-      <c r="B65" s="14"/>
-      <c r="C65" s="23"/>
-      <c r="D65" s="14"/>
-      <c r="E65" s="17"/>
-      <c r="F65" s="20"/>
+      <c r="A65" s="14"/>
+      <c r="B65" s="17"/>
+      <c r="C65" s="11"/>
+      <c r="D65" s="17"/>
+      <c r="E65" s="20"/>
+      <c r="F65" s="23"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B66" s="6" t="s">
+      <c r="B66" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="C66" s="21" t="s">
+      <c r="C66" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="D66" s="6" t="s">
+      <c r="D66" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="E66" s="15" t="s">
+      <c r="E66" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F66" s="18" t="s">
+      <c r="F66" s="21" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="7"/>
-      <c r="B67" s="13"/>
-      <c r="C67" s="22"/>
-      <c r="D67" s="13"/>
-      <c r="E67" s="16"/>
-      <c r="F67" s="19"/>
+      <c r="A67" s="13"/>
+      <c r="B67" s="16"/>
+      <c r="C67" s="10"/>
+      <c r="D67" s="16"/>
+      <c r="E67" s="19"/>
+      <c r="F67" s="22"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="7"/>
-      <c r="B68" s="13"/>
-      <c r="C68" s="22"/>
-      <c r="D68" s="13"/>
-      <c r="E68" s="16"/>
-      <c r="F68" s="19"/>
+      <c r="A68" s="13"/>
+      <c r="B68" s="16"/>
+      <c r="C68" s="10"/>
+      <c r="D68" s="16"/>
+      <c r="E68" s="19"/>
+      <c r="F68" s="22"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="8"/>
-      <c r="B69" s="14"/>
-      <c r="C69" s="23"/>
-      <c r="D69" s="14"/>
-      <c r="E69" s="17"/>
-      <c r="F69" s="20"/>
+      <c r="A69" s="14"/>
+      <c r="B69" s="17"/>
+      <c r="C69" s="11"/>
+      <c r="D69" s="17"/>
+      <c r="E69" s="20"/>
+      <c r="F69" s="23"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="B70" s="6" t="s">
+      <c r="B70" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="C70" s="6" t="s">
+      <c r="C70" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="D70" s="6" t="s">
+      <c r="D70" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="E70" s="15" t="s">
+      <c r="E70" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F70" s="9" t="s">
+      <c r="F70" s="31" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="7"/>
-      <c r="B71" s="13"/>
-      <c r="C71" s="7"/>
-      <c r="D71" s="13"/>
-      <c r="E71" s="16"/>
-      <c r="F71" s="10"/>
+      <c r="A71" s="13"/>
+      <c r="B71" s="16"/>
+      <c r="C71" s="13"/>
+      <c r="D71" s="16"/>
+      <c r="E71" s="19"/>
+      <c r="F71" s="32"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="7"/>
-      <c r="B72" s="13"/>
-      <c r="C72" s="7"/>
-      <c r="D72" s="13"/>
-      <c r="E72" s="16"/>
-      <c r="F72" s="10"/>
+      <c r="A72" s="13"/>
+      <c r="B72" s="16"/>
+      <c r="C72" s="13"/>
+      <c r="D72" s="16"/>
+      <c r="E72" s="19"/>
+      <c r="F72" s="32"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="8"/>
-      <c r="B73" s="14"/>
-      <c r="C73" s="8"/>
-      <c r="D73" s="14"/>
-      <c r="E73" s="17"/>
-      <c r="F73" s="11"/>
+      <c r="A73" s="14"/>
+      <c r="B73" s="17"/>
+      <c r="C73" s="14"/>
+      <c r="D73" s="17"/>
+      <c r="E73" s="20"/>
+      <c r="F73" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="114">
-    <mergeCell ref="F42:F45"/>
-    <mergeCell ref="C42:C45"/>
-    <mergeCell ref="A46:A49"/>
-    <mergeCell ref="B46:B49"/>
-    <mergeCell ref="C46:C49"/>
-    <mergeCell ref="D46:D49"/>
-    <mergeCell ref="E46:E49"/>
-    <mergeCell ref="F46:F49"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="B42:B45"/>
-    <mergeCell ref="D42:D45"/>
-    <mergeCell ref="E42:E45"/>
-    <mergeCell ref="E30:E33"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="C26:C29"/>
-    <mergeCell ref="D18:D21"/>
-    <mergeCell ref="E18:E21"/>
-    <mergeCell ref="E14:E17"/>
-    <mergeCell ref="F14:F17"/>
-    <mergeCell ref="D14:D17"/>
-    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="H14:H17"/>
+    <mergeCell ref="H18:H21"/>
+    <mergeCell ref="F70:F73"/>
+    <mergeCell ref="A70:A73"/>
+    <mergeCell ref="B70:B73"/>
+    <mergeCell ref="C70:C73"/>
+    <mergeCell ref="D70:D73"/>
+    <mergeCell ref="E70:E73"/>
+    <mergeCell ref="F62:F65"/>
+    <mergeCell ref="A66:A69"/>
+    <mergeCell ref="B66:B69"/>
+    <mergeCell ref="C66:C69"/>
+    <mergeCell ref="D66:D69"/>
+    <mergeCell ref="E66:E69"/>
+    <mergeCell ref="F66:F69"/>
+    <mergeCell ref="A62:A65"/>
+    <mergeCell ref="B62:B65"/>
+    <mergeCell ref="C62:C65"/>
+    <mergeCell ref="D62:D65"/>
+    <mergeCell ref="E62:E65"/>
+    <mergeCell ref="F58:F61"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="H2:H5"/>
+    <mergeCell ref="H6:H9"/>
+    <mergeCell ref="A58:A61"/>
+    <mergeCell ref="B58:B61"/>
+    <mergeCell ref="C58:C61"/>
+    <mergeCell ref="D58:D61"/>
+    <mergeCell ref="E58:E61"/>
+    <mergeCell ref="F50:F53"/>
+    <mergeCell ref="A54:A57"/>
+    <mergeCell ref="B54:B57"/>
+    <mergeCell ref="C54:C57"/>
+    <mergeCell ref="D54:D57"/>
+    <mergeCell ref="E54:E57"/>
+    <mergeCell ref="F54:F57"/>
+    <mergeCell ref="A50:A53"/>
+    <mergeCell ref="B50:B53"/>
+    <mergeCell ref="C50:C53"/>
+    <mergeCell ref="D50:D53"/>
+    <mergeCell ref="E50:E53"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="D2:D5"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="F2:F5"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="F10:F13"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="F6:F9"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="E6:E9"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="F18:F21"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="C18:C19"/>
     <mergeCell ref="F38:F41"/>
     <mergeCell ref="A22:A25"/>
     <mergeCell ref="B22:B25"/>
@@ -2363,75 +2411,27 @@
     <mergeCell ref="B38:B41"/>
     <mergeCell ref="D38:D41"/>
     <mergeCell ref="C34:C37"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="F2:F5"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="F10:F13"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="D6:D9"/>
-    <mergeCell ref="F6:F9"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="E2:E5"/>
-    <mergeCell ref="E6:E9"/>
-    <mergeCell ref="E10:E13"/>
-    <mergeCell ref="F18:F21"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="H2:H5"/>
-    <mergeCell ref="H6:H9"/>
-    <mergeCell ref="A58:A61"/>
-    <mergeCell ref="B58:B61"/>
-    <mergeCell ref="C58:C61"/>
-    <mergeCell ref="D58:D61"/>
-    <mergeCell ref="E58:E61"/>
-    <mergeCell ref="F50:F53"/>
-    <mergeCell ref="A54:A57"/>
-    <mergeCell ref="B54:B57"/>
-    <mergeCell ref="C54:C57"/>
-    <mergeCell ref="D54:D57"/>
-    <mergeCell ref="E54:E57"/>
-    <mergeCell ref="F54:F57"/>
-    <mergeCell ref="A50:A53"/>
-    <mergeCell ref="B50:B53"/>
-    <mergeCell ref="C50:C53"/>
-    <mergeCell ref="D50:D53"/>
-    <mergeCell ref="E50:E53"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="D2:D5"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="H14:H17"/>
-    <mergeCell ref="H18:H21"/>
-    <mergeCell ref="F70:F73"/>
-    <mergeCell ref="A70:A73"/>
-    <mergeCell ref="B70:B73"/>
-    <mergeCell ref="C70:C73"/>
-    <mergeCell ref="D70:D73"/>
-    <mergeCell ref="E70:E73"/>
-    <mergeCell ref="F62:F65"/>
-    <mergeCell ref="A66:A69"/>
-    <mergeCell ref="B66:B69"/>
-    <mergeCell ref="C66:C69"/>
-    <mergeCell ref="D66:D69"/>
-    <mergeCell ref="E66:E69"/>
-    <mergeCell ref="F66:F69"/>
-    <mergeCell ref="A62:A65"/>
-    <mergeCell ref="B62:B65"/>
-    <mergeCell ref="C62:C65"/>
-    <mergeCell ref="D62:D65"/>
-    <mergeCell ref="E62:E65"/>
-    <mergeCell ref="F58:F61"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="E30:E33"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="C26:C29"/>
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="E18:E21"/>
+    <mergeCell ref="E14:E17"/>
+    <mergeCell ref="F14:F17"/>
+    <mergeCell ref="D14:D17"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="F42:F45"/>
+    <mergeCell ref="C42:C45"/>
+    <mergeCell ref="A46:A49"/>
+    <mergeCell ref="B46:B49"/>
+    <mergeCell ref="C46:C49"/>
+    <mergeCell ref="D46:D49"/>
+    <mergeCell ref="E46:E49"/>
+    <mergeCell ref="F46:F49"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="B42:B45"/>
+    <mergeCell ref="D42:D45"/>
+    <mergeCell ref="E42:E45"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Mejora de navegación + ToDo actualizado
</commit_message>
<xml_diff>
--- a/ToDo/Product Backlog.xlsx
+++ b/ToDo/Product Backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juana\Escritorio\UNI\Tercero\Segundo Cuatrimestre\TaW\ArkhamMovies\ToDo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vital\Documents\GitHub\ArkhamMovies\ToDo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71B5CC9C-2DC2-4558-8643-D65C899E572E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD95F98-1F8D-4174-8166-4CF051CDB846}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{391AEB77-1329-4C84-A561-AE54ADC33E64}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{391AEB77-1329-4C84-A561-AE54ADC33E64}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="93">
   <si>
     <t>ID</t>
   </si>
@@ -412,9 +412,6 @@
     <t>Implementar la creación de un top de películas de un usuario.</t>
   </si>
   <si>
-    <t>Implementar la representación de dicho top según el orden del usuario.</t>
-  </si>
-  <si>
     <t>Implementar la representación de un top de películas según su nota.</t>
   </si>
   <si>
@@ -513,9 +510,6 @@
   </si>
   <si>
     <t>Hecho</t>
-  </si>
-  <si>
-    <t>Pendiente orden personalizado</t>
   </si>
   <si>
     <t>US11</t>
@@ -839,6 +833,64 @@
   </si>
   <si>
     <t>Arreglar los botones de volver o quitarlos (como ya se puede navegar con el header realmente no harían tanta falta)</t>
+  </si>
+  <si>
+    <r>
+      <t>Implementar la representación de dicho top según el orden del usuario. (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>No se va a hacer debido a la bd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>US19</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Como </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Usuario</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, quiero poder ver las palabras clave de las películas</t>
+    </r>
+  </si>
+  <si>
+    <t>Añadir palabras clave en películas</t>
   </si>
 </sst>
 </file>
@@ -1023,7 +1075,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1038,13 +1090,97 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1056,110 +1192,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1495,22 +1529,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D14C92F-3F4B-401B-9B84-B21C184BF8CD}">
-  <dimension ref="A1:H73"/>
+  <dimension ref="A1:H77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="34.109375" customWidth="1"/>
-    <col min="3" max="3" width="66.88671875" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" customWidth="1"/>
-    <col min="6" max="6" width="13.88671875" customWidth="1"/>
-    <col min="8" max="8" width="33.5546875" customWidth="1"/>
+    <col min="2" max="2" width="34.140625" customWidth="1"/>
+    <col min="3" max="3" width="66.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" customWidth="1"/>
+    <col min="8" max="8" width="33.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1530,932 +1564,939 @@
         <v>4</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="13"/>
+      <c r="H2" s="31" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
       <c r="B3" s="16"/>
       <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="16"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="26"/>
-      <c r="H3" s="7"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="13"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="10"/>
+      <c r="H3" s="13"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
       <c r="B4" s="16"/>
       <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="16"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="26"/>
-      <c r="H4" s="7"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="14"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="10"/>
+      <c r="H4" s="13"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="8"/>
       <c r="B5" s="17"/>
       <c r="C5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="17"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="27"/>
-      <c r="H5" s="8"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" s="15" t="s">
+      <c r="E5" s="30"/>
+      <c r="F5" s="11"/>
+      <c r="H5" s="14"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="29" t="s">
+      <c r="E6" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="H6" s="15" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="13"/>
+      <c r="F6" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
       <c r="B7" s="16"/>
-      <c r="C7" s="28"/>
+      <c r="C7" s="40"/>
       <c r="D7" s="16"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="26"/>
-      <c r="H7" s="13"/>
-    </row>
-    <row r="8" spans="1:8" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="13"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="10"/>
+      <c r="H7" s="7"/>
+    </row>
+    <row r="8" spans="1:8" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
       <c r="B8" s="16"/>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D8" s="16"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="26"/>
-      <c r="H8" s="13"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="14"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="10"/>
+      <c r="H8" s="7"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="8"/>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="27"/>
-      <c r="H9" s="14"/>
-    </row>
-    <row r="10" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" s="15" t="s">
+      <c r="E9" s="30"/>
+      <c r="F9" s="11"/>
+      <c r="H9" s="8"/>
+    </row>
+    <row r="10" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="29" t="s">
+      <c r="E10" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="25" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="13"/>
+      <c r="F10" s="9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
       <c r="B11" s="16"/>
-      <c r="C11" s="28"/>
+      <c r="C11" s="40"/>
       <c r="D11" s="16"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="26"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="13"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="10"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
       <c r="B12" s="16"/>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="6" t="s">
         <v>22</v>
       </c>
       <c r="D12" s="16"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="26"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="14"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="10"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
       <c r="B13" s="17"/>
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="27"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="11"/>
       <c r="H13" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="H14" s="31" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="10"/>
+      <c r="H15" s="13"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="7"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="16"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="10"/>
+      <c r="H16" s="13"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="11"/>
+      <c r="H17" s="14"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="H18" s="31" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="15" t="s">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="7"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="10"/>
+      <c r="H19" s="13"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="7"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="16"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="10"/>
+      <c r="H20" s="13"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="8"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="11"/>
+      <c r="H21" s="14"/>
+    </row>
+    <row r="22" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="29" t="s">
+      <c r="E22" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="13"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="26"/>
-      <c r="H15" s="7"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="13"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="16"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="26"/>
-      <c r="H16" s="7"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="14"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="27"/>
-      <c r="H17" s="8"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="B18" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="E18" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="H18" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="13"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="32"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="26"/>
-      <c r="H19" s="7"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="13"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="D20" s="16"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="26"/>
-      <c r="H20" s="7"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="14"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="32"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="27"/>
-      <c r="H21" s="8"/>
-    </row>
-    <row r="22" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="E22" s="29" t="s">
-        <v>12</v>
-      </c>
       <c r="F22" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="H22" s="44" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="13"/>
+        <v>52</v>
+      </c>
+      <c r="H22" s="31" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="7"/>
       <c r="B23" s="16"/>
       <c r="C23" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D23" s="16"/>
-      <c r="E23" s="30"/>
+      <c r="E23" s="29"/>
       <c r="F23" s="22"/>
-      <c r="H23" s="45"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="13"/>
+      <c r="H23" s="13"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="7"/>
       <c r="B24" s="16"/>
       <c r="C24" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D24" s="16"/>
-      <c r="E24" s="30"/>
+      <c r="E24" s="29"/>
       <c r="F24" s="22"/>
-      <c r="H24" s="45"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="14"/>
+      <c r="H24" s="13"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="8"/>
       <c r="B25" s="17"/>
       <c r="C25" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D25" s="17"/>
-      <c r="E25" s="31"/>
+      <c r="E25" s="30"/>
       <c r="F25" s="23"/>
-      <c r="H25" s="46"/>
-    </row>
-    <row r="26" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="12" t="s">
+      <c r="H25" s="14"/>
+    </row>
+    <row r="26" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E26" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" s="37" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="7"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="38"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="7"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="38"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="8"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="39"/>
+    </row>
+    <row r="30" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B26" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="D26" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="E26" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="F26" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="13"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="10"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="13"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="10"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="14"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="11"/>
-    </row>
-    <row r="30" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>85</v>
+      <c r="B30" s="31" t="s">
+        <v>83</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D30" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="E30" s="41" t="s">
+      <c r="E30" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="F30" s="38" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="7"/>
-      <c r="B31" s="36"/>
+      <c r="F30" s="34" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="13"/>
+      <c r="B31" s="32"/>
       <c r="C31" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D31" s="36"/>
-      <c r="E31" s="42"/>
-      <c r="F31" s="39"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="7"/>
-      <c r="B32" s="36"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="25"/>
+      <c r="F31" s="35"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="13"/>
+      <c r="B32" s="32"/>
       <c r="C32" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D32" s="36"/>
-      <c r="E32" s="42"/>
-      <c r="F32" s="39"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="8"/>
-      <c r="B33" s="37"/>
+      <c r="D32" s="32"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="35"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="14"/>
+      <c r="B33" s="33"/>
       <c r="C33" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="D33" s="37"/>
-      <c r="E33" s="43"/>
-      <c r="F33" s="40"/>
-    </row>
-    <row r="34" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B34" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="D33" s="33"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="36"/>
+    </row>
+    <row r="34" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B34" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C34" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="D34" s="15" t="s">
-        <v>41</v>
+      <c r="C34" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>40</v>
       </c>
       <c r="E34" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F34" s="25" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="13"/>
+      <c r="F34" s="9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="7"/>
       <c r="B35" s="16"/>
-      <c r="C35" s="7"/>
+      <c r="C35" s="13"/>
       <c r="D35" s="16"/>
       <c r="E35" s="19"/>
-      <c r="F35" s="26"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="13"/>
+      <c r="F35" s="10"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="7"/>
       <c r="B36" s="16"/>
-      <c r="C36" s="7"/>
+      <c r="C36" s="13"/>
       <c r="D36" s="16"/>
       <c r="E36" s="19"/>
-      <c r="F36" s="26"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="14"/>
+      <c r="F36" s="10"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="8"/>
       <c r="B37" s="17"/>
-      <c r="C37" s="8"/>
+      <c r="C37" s="14"/>
       <c r="D37" s="17"/>
       <c r="E37" s="20"/>
-      <c r="F37" s="27"/>
-    </row>
-    <row r="38" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="B38" s="15" t="s">
+      <c r="F37" s="11"/>
+    </row>
+    <row r="38" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B38" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C38" s="24" t="s">
+      <c r="C38" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D38" s="15" t="s">
+      <c r="D38" s="6" t="s">
         <v>28</v>
       </c>
       <c r="E38" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F38" s="33" t="s">
-        <v>54</v>
+      <c r="F38" s="9" t="s">
+        <v>52</v>
       </c>
       <c r="G38" s="3"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="13"/>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="7"/>
       <c r="B39" s="16"/>
-      <c r="C39" s="8"/>
+      <c r="C39" s="14"/>
       <c r="D39" s="16"/>
       <c r="E39" s="19"/>
-      <c r="F39" s="34"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="13"/>
+      <c r="F39" s="10"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="7"/>
       <c r="B40" s="16"/>
-      <c r="C40" s="12" t="s">
-        <v>34</v>
+      <c r="C40" s="6" t="s">
+        <v>89</v>
       </c>
       <c r="D40" s="16"/>
       <c r="E40" s="19"/>
-      <c r="F40" s="34"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="14"/>
+      <c r="F40" s="10"/>
+    </row>
+    <row r="41" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="8"/>
       <c r="B41" s="17"/>
-      <c r="C41" s="14"/>
+      <c r="C41" s="17"/>
       <c r="D41" s="17"/>
       <c r="E41" s="20"/>
-      <c r="F41" s="35"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="B42" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="C42" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="D42" s="15" t="s">
+      <c r="F41" s="11"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D42" s="6" t="s">
         <v>28</v>
       </c>
       <c r="E42" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F42" s="25" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="13"/>
+      <c r="F42" s="9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="7"/>
       <c r="B43" s="16"/>
-      <c r="C43" s="7"/>
+      <c r="C43" s="13"/>
       <c r="D43" s="16"/>
       <c r="E43" s="19"/>
-      <c r="F43" s="26"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="13"/>
+      <c r="F43" s="10"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="7"/>
       <c r="B44" s="16"/>
-      <c r="C44" s="7"/>
+      <c r="C44" s="13"/>
       <c r="D44" s="16"/>
       <c r="E44" s="19"/>
-      <c r="F44" s="26"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="14"/>
+      <c r="F44" s="10"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="8"/>
       <c r="B45" s="17"/>
-      <c r="C45" s="8"/>
+      <c r="C45" s="14"/>
       <c r="D45" s="17"/>
       <c r="E45" s="20"/>
-      <c r="F45" s="27"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="B46" s="15" t="s">
+      <c r="F45" s="11"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="C46" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="D46" s="15" t="s">
+      <c r="B46" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C46" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D46" s="6" t="s">
         <v>28</v>
       </c>
       <c r="E46" s="18" t="s">
         <v>14</v>
       </c>
       <c r="F46" s="21" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="13"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="7"/>
       <c r="B47" s="16"/>
-      <c r="C47" s="7"/>
+      <c r="C47" s="13"/>
       <c r="D47" s="16"/>
       <c r="E47" s="19"/>
       <c r="F47" s="22"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="13"/>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="7"/>
       <c r="B48" s="16"/>
-      <c r="C48" s="7"/>
+      <c r="C48" s="13"/>
       <c r="D48" s="16"/>
       <c r="E48" s="19"/>
       <c r="F48" s="22"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" s="14"/>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="8"/>
       <c r="B49" s="17"/>
-      <c r="C49" s="8"/>
+      <c r="C49" s="14"/>
       <c r="D49" s="17"/>
       <c r="E49" s="20"/>
       <c r="F49" s="23"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="B50" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="C50" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="D50" s="15" t="s">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C50" s="12" t="s">
         <v>61</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="E50" s="18" t="s">
         <v>14</v>
       </c>
       <c r="F50" s="21" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="13"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="7"/>
       <c r="B51" s="16"/>
-      <c r="C51" s="7"/>
+      <c r="C51" s="13"/>
       <c r="D51" s="16"/>
       <c r="E51" s="19"/>
       <c r="F51" s="22"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" s="13"/>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="7"/>
       <c r="B52" s="16"/>
-      <c r="C52" s="7"/>
+      <c r="C52" s="13"/>
       <c r="D52" s="16"/>
       <c r="E52" s="19"/>
       <c r="F52" s="22"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" s="14"/>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="8"/>
       <c r="B53" s="17"/>
-      <c r="C53" s="8"/>
+      <c r="C53" s="14"/>
       <c r="D53" s="17"/>
       <c r="E53" s="20"/>
       <c r="F53" s="23"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="B54" s="15" t="s">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C54" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="C54" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="D54" s="15" t="s">
-        <v>61</v>
+      <c r="D54" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="E54" s="18" t="s">
         <v>14</v>
       </c>
       <c r="F54" s="21" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" s="13"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="7"/>
       <c r="B55" s="16"/>
-      <c r="C55" s="7"/>
+      <c r="C55" s="13"/>
       <c r="D55" s="16"/>
       <c r="E55" s="19"/>
       <c r="F55" s="22"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" s="13"/>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="7"/>
       <c r="B56" s="16"/>
-      <c r="C56" s="7"/>
+      <c r="C56" s="13"/>
       <c r="D56" s="16"/>
       <c r="E56" s="19"/>
       <c r="F56" s="22"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A57" s="14"/>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="8"/>
       <c r="B57" s="17"/>
-      <c r="C57" s="8"/>
+      <c r="C57" s="14"/>
       <c r="D57" s="17"/>
       <c r="E57" s="20"/>
       <c r="F57" s="23"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="B58" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="C58" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="D58" s="15" t="s">
-        <v>61</v>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C58" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="E58" s="18" t="s">
         <v>14</v>
       </c>
       <c r="F58" s="21" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" s="13"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="7"/>
       <c r="B59" s="16"/>
-      <c r="C59" s="7"/>
+      <c r="C59" s="13"/>
       <c r="D59" s="16"/>
       <c r="E59" s="19"/>
       <c r="F59" s="22"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A60" s="13"/>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="7"/>
       <c r="B60" s="16"/>
-      <c r="C60" s="7"/>
+      <c r="C60" s="13"/>
       <c r="D60" s="16"/>
       <c r="E60" s="19"/>
       <c r="F60" s="22"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A61" s="14"/>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="8"/>
       <c r="B61" s="17"/>
-      <c r="C61" s="8"/>
+      <c r="C61" s="14"/>
       <c r="D61" s="17"/>
       <c r="E61" s="20"/>
       <c r="F61" s="23"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="B62" s="15" t="s">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="C62" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="D62" s="15" t="s">
-        <v>61</v>
+      <c r="B62" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C62" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="E62" s="18" t="s">
         <v>14</v>
       </c>
       <c r="F62" s="21" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A63" s="13"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="7"/>
       <c r="B63" s="16"/>
-      <c r="C63" s="7"/>
+      <c r="C63" s="13"/>
       <c r="D63" s="16"/>
       <c r="E63" s="19"/>
       <c r="F63" s="22"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A64" s="13"/>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="7"/>
       <c r="B64" s="16"/>
-      <c r="C64" s="7"/>
+      <c r="C64" s="13"/>
       <c r="D64" s="16"/>
       <c r="E64" s="19"/>
       <c r="F64" s="22"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A65" s="14"/>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="8"/>
       <c r="B65" s="17"/>
-      <c r="C65" s="8"/>
+      <c r="C65" s="14"/>
       <c r="D65" s="17"/>
       <c r="E65" s="20"/>
       <c r="F65" s="23"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A66" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="B66" s="15" t="s">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="C66" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D66" s="15" t="s">
+      <c r="B66" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C66" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="D66" s="6" t="s">
         <v>28</v>
       </c>
       <c r="E66" s="18" t="s">
         <v>14</v>
       </c>
       <c r="F66" s="21" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A67" s="13"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="7"/>
       <c r="B67" s="16"/>
-      <c r="C67" s="7"/>
+      <c r="C67" s="13"/>
       <c r="D67" s="16"/>
       <c r="E67" s="19"/>
       <c r="F67" s="22"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A68" s="13"/>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="7"/>
       <c r="B68" s="16"/>
-      <c r="C68" s="7"/>
+      <c r="C68" s="13"/>
       <c r="D68" s="16"/>
       <c r="E68" s="19"/>
       <c r="F68" s="22"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A69" s="14"/>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="8"/>
       <c r="B69" s="17"/>
-      <c r="C69" s="8"/>
+      <c r="C69" s="14"/>
       <c r="D69" s="17"/>
       <c r="E69" s="20"/>
       <c r="F69" s="23"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A70" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="B70" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="C70" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="D70" s="15" t="s">
-        <v>41</v>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C70" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>40</v>
       </c>
       <c r="E70" s="18" t="s">
         <v>14</v>
       </c>
       <c r="F70" s="21" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A71" s="13"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="7"/>
       <c r="B71" s="16"/>
-      <c r="C71" s="7"/>
+      <c r="C71" s="13"/>
       <c r="D71" s="16"/>
       <c r="E71" s="19"/>
       <c r="F71" s="22"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A72" s="13"/>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="7"/>
       <c r="B72" s="16"/>
-      <c r="C72" s="7"/>
+      <c r="C72" s="13"/>
       <c r="D72" s="16"/>
       <c r="E72" s="19"/>
       <c r="F72" s="22"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A73" s="14"/>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="8"/>
       <c r="B73" s="17"/>
-      <c r="C73" s="8"/>
+      <c r="C73" s="14"/>
       <c r="D73" s="17"/>
       <c r="E73" s="20"/>
       <c r="F73" s="23"/>
     </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="B74" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C74" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="D74" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E74" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F74" s="21" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="7"/>
+      <c r="B75" s="16"/>
+      <c r="C75" s="13"/>
+      <c r="D75" s="16"/>
+      <c r="E75" s="19"/>
+      <c r="F75" s="22"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="7"/>
+      <c r="B76" s="16"/>
+      <c r="C76" s="13"/>
+      <c r="D76" s="16"/>
+      <c r="E76" s="19"/>
+      <c r="F76" s="22"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="8"/>
+      <c r="B77" s="17"/>
+      <c r="C77" s="14"/>
+      <c r="D77" s="17"/>
+      <c r="E77" s="20"/>
+      <c r="F77" s="23"/>
+    </row>
   </sheetData>
-  <mergeCells count="115">
-    <mergeCell ref="H22:H25"/>
-    <mergeCell ref="F42:F45"/>
-    <mergeCell ref="C42:C45"/>
-    <mergeCell ref="A46:A49"/>
-    <mergeCell ref="B46:B49"/>
-    <mergeCell ref="C46:C49"/>
-    <mergeCell ref="D46:D49"/>
-    <mergeCell ref="E46:E49"/>
-    <mergeCell ref="F46:F49"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="B42:B45"/>
-    <mergeCell ref="D42:D45"/>
-    <mergeCell ref="E42:E45"/>
-    <mergeCell ref="E30:E33"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="C26:C29"/>
-    <mergeCell ref="D18:D21"/>
-    <mergeCell ref="E18:E21"/>
-    <mergeCell ref="E14:E17"/>
-    <mergeCell ref="F14:F17"/>
-    <mergeCell ref="D14:D17"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="F38:F41"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="D22:D25"/>
-    <mergeCell ref="F22:F25"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="F34:F37"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="F30:F33"/>
-    <mergeCell ref="E34:E37"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="F26:F29"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="E22:E25"/>
-    <mergeCell ref="E26:E29"/>
-    <mergeCell ref="E38:E41"/>
-    <mergeCell ref="B38:B41"/>
-    <mergeCell ref="D38:D41"/>
-    <mergeCell ref="C34:C37"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="F2:F5"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="F10:F13"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="D6:D9"/>
-    <mergeCell ref="F6:F9"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="E2:E5"/>
-    <mergeCell ref="E6:E9"/>
-    <mergeCell ref="E10:E13"/>
-    <mergeCell ref="F18:F21"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="C18:C19"/>
+  <mergeCells count="121">
+    <mergeCell ref="A74:A77"/>
+    <mergeCell ref="B74:B77"/>
+    <mergeCell ref="C74:C77"/>
+    <mergeCell ref="D74:D77"/>
+    <mergeCell ref="E74:E77"/>
+    <mergeCell ref="F74:F77"/>
+    <mergeCell ref="H14:H17"/>
+    <mergeCell ref="H18:H21"/>
+    <mergeCell ref="F70:F73"/>
+    <mergeCell ref="A70:A73"/>
+    <mergeCell ref="B70:B73"/>
+    <mergeCell ref="C70:C73"/>
+    <mergeCell ref="D70:D73"/>
+    <mergeCell ref="E70:E73"/>
+    <mergeCell ref="F62:F65"/>
+    <mergeCell ref="A66:A69"/>
+    <mergeCell ref="B66:B69"/>
+    <mergeCell ref="C66:C69"/>
+    <mergeCell ref="D66:D69"/>
+    <mergeCell ref="E66:E69"/>
+    <mergeCell ref="F66:F69"/>
+    <mergeCell ref="A62:A65"/>
+    <mergeCell ref="B62:B65"/>
+    <mergeCell ref="C62:C65"/>
+    <mergeCell ref="D62:D65"/>
+    <mergeCell ref="E62:E65"/>
+    <mergeCell ref="F58:F61"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B14:B17"/>
     <mergeCell ref="H2:H5"/>
     <mergeCell ref="H6:H9"/>
     <mergeCell ref="A58:A61"/>
@@ -2480,30 +2521,73 @@
     <mergeCell ref="D2:D5"/>
     <mergeCell ref="A38:A41"/>
     <mergeCell ref="A14:A17"/>
-    <mergeCell ref="H14:H17"/>
-    <mergeCell ref="H18:H21"/>
-    <mergeCell ref="F70:F73"/>
-    <mergeCell ref="A70:A73"/>
-    <mergeCell ref="B70:B73"/>
-    <mergeCell ref="C70:C73"/>
-    <mergeCell ref="D70:D73"/>
-    <mergeCell ref="E70:E73"/>
-    <mergeCell ref="F62:F65"/>
-    <mergeCell ref="A66:A69"/>
-    <mergeCell ref="B66:B69"/>
-    <mergeCell ref="C66:C69"/>
-    <mergeCell ref="D66:D69"/>
-    <mergeCell ref="E66:E69"/>
-    <mergeCell ref="F66:F69"/>
-    <mergeCell ref="A62:A65"/>
-    <mergeCell ref="B62:B65"/>
-    <mergeCell ref="C62:C65"/>
-    <mergeCell ref="D62:D65"/>
-    <mergeCell ref="E62:E65"/>
-    <mergeCell ref="F58:F61"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="F2:F5"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="F10:F13"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="F6:F9"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="E6:E9"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="F18:F21"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="C26:C29"/>
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="E18:E21"/>
+    <mergeCell ref="E14:E17"/>
+    <mergeCell ref="F14:F17"/>
+    <mergeCell ref="D14:D17"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="F38:F41"/>
+    <mergeCell ref="D22:D25"/>
+    <mergeCell ref="F22:F25"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="F34:F37"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="F30:F33"/>
+    <mergeCell ref="E34:E37"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="F26:F29"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="E22:E25"/>
+    <mergeCell ref="E26:E29"/>
+    <mergeCell ref="E38:E41"/>
+    <mergeCell ref="D38:D41"/>
+    <mergeCell ref="H22:H25"/>
+    <mergeCell ref="F42:F45"/>
+    <mergeCell ref="C42:C45"/>
+    <mergeCell ref="A46:A49"/>
+    <mergeCell ref="B46:B49"/>
+    <mergeCell ref="C46:C49"/>
+    <mergeCell ref="D46:D49"/>
+    <mergeCell ref="E46:E49"/>
+    <mergeCell ref="F46:F49"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="B42:B45"/>
+    <mergeCell ref="D42:D45"/>
+    <mergeCell ref="E42:E45"/>
+    <mergeCell ref="E30:E33"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="C34:C37"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Orden scripts, comentarios quitados, ToDO casi hecha e imports innecesarios fuera
</commit_message>
<xml_diff>
--- a/ToDo/Product Backlog.xlsx
+++ b/ToDo/Product Backlog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vital\Documents\GitHub\ArkhamMovies\ToDo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minie\Desktop\UMA\Tercer Curso\2do cuatrimestre\Tecnologías de Aplicaciones Web\Trabajo en grupo\ArkhamMovies\ToDo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94F68D22-7540-415E-A4B9-6046640D9724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0854F252-3102-434A-B6B0-B693111DD8B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{391AEB77-1329-4C84-A561-AE54ADC33E64}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="92">
   <si>
     <t>ID</t>
   </si>
@@ -109,8 +109,14 @@
     <t>Implementar la consulta de peticiones.</t>
   </si>
   <si>
-    <r>
-      <t>Implementar envío de mensajes para justificar el veto. (</t>
+    <t>Implementar la confirmación de una petición.</t>
+  </si>
+  <si>
+    <t>Implementar la desactivación / borrado de una cuenta usuario.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Como </t>
     </r>
     <r>
       <rPr>
@@ -121,38 +127,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>opcional</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <t>Implementar la confirmación de una petición.</t>
-  </si>
-  <si>
-    <t>Implementar la desactivación / borrado de una cuenta usuario.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Como </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>Administrador</t>
     </r>
     <r>
@@ -168,32 +142,6 @@
   </si>
   <si>
     <t>Implementar el borrado de una reseña.</t>
-  </si>
-  <si>
-    <r>
-      <t>Implementar envío de mensajes para justificar el borrado. (</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>opcional</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
   </si>
   <si>
     <r>
@@ -820,9 +768,6 @@
     </r>
   </si>
   <si>
-    <t>NO</t>
-  </si>
-  <si>
     <t>Implementar la representación visual del análisis/estadísticas de la aplicación.</t>
   </si>
   <si>
@@ -832,6 +777,90 @@
     <t>Arreglar los botones de volver o quitarlos (como ya se puede navegar con el header realmente no harían tanta falta)</t>
   </si>
   <si>
+    <t>US19</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Como </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Usuario</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, quiero poder ver las palabras clave de las películas</t>
+    </r>
+  </si>
+  <si>
+    <t>Añadir palabras clave en películas</t>
+  </si>
+  <si>
+    <r>
+      <t>Implementar envío de mensajes para justificar el veto. (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>opcional</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Implementar envío de mensajes para justificar el borrado. (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>opcional</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
     <r>
       <t>Implementar la representación de dicho top según el orden del usuario. (</t>
     </r>
@@ -858,43 +887,14 @@
     </r>
   </si>
   <si>
-    <t>US19</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Como </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Usuario</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, quiero poder ver las palabras clave de las películas</t>
-    </r>
-  </si>
-  <si>
-    <t>Añadir palabras clave en películas</t>
+    <t>Descartado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -942,6 +942,13 @@
     <font>
       <b/>
       <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -1066,14 +1073,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1081,6 +1085,18 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1099,15 +1115,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1126,20 +1133,29 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1150,31 +1166,31 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1511,10 +1527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D14C92F-3F4B-401B-9B84-B21C184BF8CD}">
-  <dimension ref="A1:H77"/>
+  <dimension ref="A1:I77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="C40" sqref="C40:C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1526,7 +1542,7 @@
     <col min="8" max="8" width="33.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1545,910 +1561,1035 @@
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="10"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="13"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="7"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="7"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="13"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="7"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="7"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="11"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="14"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="8"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="8"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H6" s="12" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+    <row r="7" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="10"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="7"/>
+      <c r="H7" s="10"/>
+    </row>
+    <row r="8" spans="1:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="10"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="D8" s="13"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="7"/>
+      <c r="H8" s="10"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="11"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="8"/>
+      <c r="H9" s="11"/>
+    </row>
+    <row r="10" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B10" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="10"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="7"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="10"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="D12" s="13"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="11"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="8"/>
+      <c r="H13" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="E2" s="26" t="s">
+      <c r="C14" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="H2" s="12" t="s">
+      <c r="F14" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H14" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="10"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="7"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="7"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="10"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="13"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="7"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="7"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="11"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="8"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="8"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H18" s="35" t="s">
+        <v>79</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="10"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="7"/>
+      <c r="H19" s="40"/>
+      <c r="I19" s="7"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="10"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="13"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="7"/>
+      <c r="H20" s="40"/>
+      <c r="I20" s="7"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="11"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="8"/>
+      <c r="H21" s="37"/>
+      <c r="I21" s="8"/>
+    </row>
+    <row r="22" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="H22" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="10"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" s="13"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="19"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="7"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="10"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="13"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="19"/>
+      <c r="H24" s="40"/>
+      <c r="I24" s="7"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="11"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" s="14"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="20"/>
+      <c r="H25" s="37"/>
+      <c r="I25" s="8"/>
+    </row>
+    <row r="26" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="D26" s="12" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="23"/>
-      <c r="H3" s="13"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="23"/>
-      <c r="H4" s="13"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="24"/>
-      <c r="H5" s="14"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="9" t="s">
+      <c r="E26" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="10"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="19"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="10"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="19"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="11"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="20"/>
+    </row>
+    <row r="30" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="23"/>
-      <c r="H7" s="7"/>
-    </row>
-    <row r="8" spans="1:8" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="9" t="s">
+      <c r="E30" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="F30" s="26" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="40"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="23"/>
-      <c r="H8" s="7"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="24"/>
-      <c r="H9" s="8"/>
-    </row>
-    <row r="10" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="22" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="23"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="23"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="24"/>
-      <c r="H13" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="H14" s="12" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="23"/>
-      <c r="H15" s="13"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="21" t="s">
+      <c r="D31" s="24"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="27"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="40"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32" s="24"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="27"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="37"/>
+      <c r="B33" s="25"/>
+      <c r="C33" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D33" s="25"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="28"/>
+    </row>
+    <row r="34" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="10"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="23"/>
-      <c r="H16" s="13"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="24"/>
-      <c r="H17" s="14"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="E18" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="F18" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="H18" s="12" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="23"/>
-      <c r="H19" s="13"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" s="10"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="23"/>
-      <c r="H20" s="13"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="24"/>
-      <c r="H21" s="14"/>
-    </row>
-    <row r="22" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E22" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="F22" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="H22" s="12" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D23" s="10"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="19"/>
-      <c r="H23" s="13"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="2" t="s">
+      <c r="C34" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="D34" s="12" t="s">
         <v>37</v>
-      </c>
-      <c r="D24" s="10"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="19"/>
-      <c r="H24" s="13"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D25" s="11"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="20"/>
-      <c r="H25" s="14"/>
-    </row>
-    <row r="26" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="E26" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="F26" s="18" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
-      <c r="B27" s="10"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="27"/>
-      <c r="F27" s="19"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="30"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="19"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="8"/>
-      <c r="B29" s="11"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="28"/>
-      <c r="F29" s="20"/>
-    </row>
-    <row r="30" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="B30" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D30" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E30" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="F30" s="32" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="13"/>
-      <c r="B31" s="30"/>
-      <c r="C31" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D31" s="30"/>
-      <c r="E31" s="36"/>
-      <c r="F31" s="33"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="13"/>
-      <c r="B32" s="30"/>
-      <c r="C32" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D32" s="30"/>
-      <c r="E32" s="36"/>
-      <c r="F32" s="33"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="14"/>
-      <c r="B33" s="31"/>
-      <c r="C33" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="D33" s="31"/>
-      <c r="E33" s="37"/>
-      <c r="F33" s="34"/>
-    </row>
-    <row r="34" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C34" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>39</v>
       </c>
       <c r="E34" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="F34" s="22" t="s">
-        <v>51</v>
+      <c r="F34" s="6" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="7"/>
-      <c r="B35" s="10"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="10"/>
+      <c r="A35" s="10"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="40"/>
+      <c r="D35" s="13"/>
       <c r="E35" s="16"/>
-      <c r="F35" s="23"/>
+      <c r="F35" s="7"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="7"/>
-      <c r="B36" s="10"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="10"/>
+      <c r="A36" s="10"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="40"/>
+      <c r="D36" s="13"/>
       <c r="E36" s="16"/>
-      <c r="F36" s="23"/>
+      <c r="F36" s="7"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="8"/>
-      <c r="B37" s="11"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="11"/>
+      <c r="A37" s="11"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="37"/>
+      <c r="D37" s="14"/>
       <c r="E37" s="17"/>
-      <c r="F37" s="24"/>
+      <c r="F37" s="8"/>
     </row>
     <row r="38" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B38" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C38" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="D38" s="9" t="s">
-        <v>27</v>
+      <c r="A38" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C38" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>25</v>
       </c>
       <c r="E38" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="F38" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="G38" s="3"/>
+      <c r="F38" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G38" s="2"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="7"/>
-      <c r="B39" s="10"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="10"/>
+      <c r="A39" s="10"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="37"/>
+      <c r="D39" s="13"/>
       <c r="E39" s="16"/>
-      <c r="F39" s="23"/>
+      <c r="F39" s="7"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="7"/>
-      <c r="B40" s="10"/>
-      <c r="C40" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="D40" s="10"/>
+      <c r="A40" s="10"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="D40" s="13"/>
       <c r="E40" s="16"/>
-      <c r="F40" s="23"/>
+      <c r="F40" s="7"/>
     </row>
     <row r="41" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="8"/>
-      <c r="B41" s="11"/>
-      <c r="C41" s="11"/>
-      <c r="D41" s="11"/>
+      <c r="A41" s="11"/>
+      <c r="B41" s="14"/>
+      <c r="C41" s="36"/>
+      <c r="D41" s="14"/>
       <c r="E41" s="17"/>
-      <c r="F41" s="24"/>
+      <c r="F41" s="8"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B42" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C42" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="D42" s="9" t="s">
-        <v>27</v>
+      <c r="A42" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B42" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C42" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="D42" s="12" t="s">
+        <v>25</v>
       </c>
       <c r="E42" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="F42" s="22" t="s">
+      <c r="F42" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="10"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="40"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="7"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="10"/>
+      <c r="B44" s="13"/>
+      <c r="C44" s="40"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="16"/>
+      <c r="F44" s="7"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="11"/>
+      <c r="B45" s="14"/>
+      <c r="C45" s="37"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="17"/>
+      <c r="F45" s="8"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B46" s="12" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="7"/>
-      <c r="B43" s="10"/>
-      <c r="C43" s="13"/>
-      <c r="D43" s="10"/>
-      <c r="E43" s="16"/>
-      <c r="F43" s="23"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="7"/>
-      <c r="B44" s="10"/>
-      <c r="C44" s="13"/>
-      <c r="D44" s="10"/>
-      <c r="E44" s="16"/>
-      <c r="F44" s="23"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="8"/>
-      <c r="B45" s="11"/>
-      <c r="C45" s="14"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="17"/>
-      <c r="F45" s="24"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B46" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="C46" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="D46" s="9" t="s">
-        <v>27</v>
+      <c r="C46" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="D46" s="12" t="s">
+        <v>25</v>
       </c>
       <c r="E46" s="15" t="s">
         <v>13</v>
       </c>
       <c r="F46" s="18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="7"/>
-      <c r="B47" s="10"/>
-      <c r="C47" s="13"/>
-      <c r="D47" s="10"/>
+      <c r="A47" s="10"/>
+      <c r="B47" s="13"/>
+      <c r="C47" s="40"/>
+      <c r="D47" s="13"/>
       <c r="E47" s="16"/>
       <c r="F47" s="19"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="7"/>
-      <c r="B48" s="10"/>
-      <c r="C48" s="13"/>
-      <c r="D48" s="10"/>
+      <c r="A48" s="10"/>
+      <c r="B48" s="13"/>
+      <c r="C48" s="40"/>
+      <c r="D48" s="13"/>
       <c r="E48" s="16"/>
       <c r="F48" s="19"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="8"/>
-      <c r="B49" s="11"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="11"/>
+      <c r="A49" s="11"/>
+      <c r="B49" s="14"/>
+      <c r="C49" s="37"/>
+      <c r="D49" s="14"/>
       <c r="E49" s="17"/>
       <c r="F49" s="20"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="B50" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C50" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D50" s="9" t="s">
+      <c r="A50" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B50" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C50" s="33" t="s">
         <v>58</v>
+      </c>
+      <c r="D50" s="12" t="s">
+        <v>56</v>
       </c>
       <c r="E50" s="15" t="s">
         <v>13</v>
       </c>
       <c r="F50" s="18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="7"/>
-      <c r="B51" s="10"/>
-      <c r="C51" s="13"/>
-      <c r="D51" s="10"/>
+      <c r="A51" s="10"/>
+      <c r="B51" s="13"/>
+      <c r="C51" s="40"/>
+      <c r="D51" s="13"/>
       <c r="E51" s="16"/>
       <c r="F51" s="19"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="7"/>
-      <c r="B52" s="10"/>
-      <c r="C52" s="13"/>
-      <c r="D52" s="10"/>
+      <c r="A52" s="10"/>
+      <c r="B52" s="13"/>
+      <c r="C52" s="40"/>
+      <c r="D52" s="13"/>
       <c r="E52" s="16"/>
       <c r="F52" s="19"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="8"/>
-      <c r="B53" s="11"/>
-      <c r="C53" s="14"/>
-      <c r="D53" s="11"/>
+      <c r="A53" s="11"/>
+      <c r="B53" s="14"/>
+      <c r="C53" s="37"/>
+      <c r="D53" s="14"/>
       <c r="E53" s="17"/>
       <c r="F53" s="20"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="B54" s="9" t="s">
+      <c r="A54" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B54" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C54" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="C54" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="D54" s="9" t="s">
-        <v>58</v>
+      <c r="D54" s="12" t="s">
+        <v>56</v>
       </c>
       <c r="E54" s="15" t="s">
         <v>13</v>
       </c>
       <c r="F54" s="18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="7"/>
-      <c r="B55" s="10"/>
-      <c r="C55" s="13"/>
-      <c r="D55" s="10"/>
+      <c r="A55" s="10"/>
+      <c r="B55" s="13"/>
+      <c r="C55" s="40"/>
+      <c r="D55" s="13"/>
       <c r="E55" s="16"/>
       <c r="F55" s="19"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="7"/>
-      <c r="B56" s="10"/>
-      <c r="C56" s="13"/>
-      <c r="D56" s="10"/>
+      <c r="A56" s="10"/>
+      <c r="B56" s="13"/>
+      <c r="C56" s="40"/>
+      <c r="D56" s="13"/>
       <c r="E56" s="16"/>
       <c r="F56" s="19"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="8"/>
-      <c r="B57" s="11"/>
-      <c r="C57" s="14"/>
-      <c r="D57" s="11"/>
+      <c r="A57" s="11"/>
+      <c r="B57" s="14"/>
+      <c r="C57" s="37"/>
+      <c r="D57" s="14"/>
       <c r="E57" s="17"/>
       <c r="F57" s="20"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="B58" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="C58" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="D58" s="9" t="s">
-        <v>58</v>
+      <c r="A58" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B58" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C58" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="D58" s="12" t="s">
+        <v>56</v>
       </c>
       <c r="E58" s="15" t="s">
         <v>13</v>
       </c>
       <c r="F58" s="18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="7"/>
-      <c r="B59" s="10"/>
-      <c r="C59" s="13"/>
-      <c r="D59" s="10"/>
+      <c r="A59" s="10"/>
+      <c r="B59" s="13"/>
+      <c r="C59" s="40"/>
+      <c r="D59" s="13"/>
       <c r="E59" s="16"/>
       <c r="F59" s="19"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="7"/>
-      <c r="B60" s="10"/>
-      <c r="C60" s="13"/>
-      <c r="D60" s="10"/>
+      <c r="A60" s="10"/>
+      <c r="B60" s="13"/>
+      <c r="C60" s="40"/>
+      <c r="D60" s="13"/>
       <c r="E60" s="16"/>
       <c r="F60" s="19"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="8"/>
-      <c r="B61" s="11"/>
-      <c r="C61" s="14"/>
-      <c r="D61" s="11"/>
+      <c r="A61" s="11"/>
+      <c r="B61" s="14"/>
+      <c r="C61" s="37"/>
+      <c r="D61" s="14"/>
       <c r="E61" s="17"/>
       <c r="F61" s="20"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="B62" s="9" t="s">
+      <c r="A62" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="C62" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="D62" s="9" t="s">
-        <v>58</v>
+      <c r="B62" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C62" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="D62" s="12" t="s">
+        <v>56</v>
       </c>
       <c r="E62" s="15" t="s">
         <v>13</v>
       </c>
       <c r="F62" s="18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="7"/>
-      <c r="B63" s="10"/>
-      <c r="C63" s="13"/>
-      <c r="D63" s="10"/>
+      <c r="A63" s="10"/>
+      <c r="B63" s="13"/>
+      <c r="C63" s="40"/>
+      <c r="D63" s="13"/>
       <c r="E63" s="16"/>
       <c r="F63" s="19"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="7"/>
-      <c r="B64" s="10"/>
-      <c r="C64" s="13"/>
-      <c r="D64" s="10"/>
+      <c r="A64" s="10"/>
+      <c r="B64" s="13"/>
+      <c r="C64" s="40"/>
+      <c r="D64" s="13"/>
       <c r="E64" s="16"/>
       <c r="F64" s="19"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="8"/>
-      <c r="B65" s="11"/>
-      <c r="C65" s="14"/>
-      <c r="D65" s="11"/>
+      <c r="A65" s="11"/>
+      <c r="B65" s="14"/>
+      <c r="C65" s="37"/>
+      <c r="D65" s="14"/>
       <c r="E65" s="17"/>
       <c r="F65" s="20"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="B66" s="9" t="s">
+      <c r="A66" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="C66" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="D66" s="9" t="s">
-        <v>27</v>
+      <c r="B66" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C66" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="D66" s="12" t="s">
+        <v>25</v>
       </c>
       <c r="E66" s="15" t="s">
         <v>13</v>
       </c>
       <c r="F66" s="18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="7"/>
-      <c r="B67" s="10"/>
-      <c r="C67" s="13"/>
-      <c r="D67" s="10"/>
+      <c r="A67" s="10"/>
+      <c r="B67" s="13"/>
+      <c r="C67" s="40"/>
+      <c r="D67" s="13"/>
       <c r="E67" s="16"/>
       <c r="F67" s="19"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="7"/>
-      <c r="B68" s="10"/>
-      <c r="C68" s="13"/>
-      <c r="D68" s="10"/>
+      <c r="A68" s="10"/>
+      <c r="B68" s="13"/>
+      <c r="C68" s="40"/>
+      <c r="D68" s="13"/>
       <c r="E68" s="16"/>
       <c r="F68" s="19"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="8"/>
-      <c r="B69" s="11"/>
-      <c r="C69" s="14"/>
-      <c r="D69" s="11"/>
+      <c r="A69" s="11"/>
+      <c r="B69" s="14"/>
+      <c r="C69" s="37"/>
+      <c r="D69" s="14"/>
       <c r="E69" s="17"/>
       <c r="F69" s="20"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B70" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="C70" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="D70" s="9" t="s">
-        <v>39</v>
+      <c r="A70" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B70" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C70" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="D70" s="12" t="s">
+        <v>37</v>
       </c>
       <c r="E70" s="15" t="s">
         <v>13</v>
       </c>
       <c r="F70" s="18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="7"/>
-      <c r="B71" s="10"/>
-      <c r="C71" s="13"/>
-      <c r="D71" s="10"/>
+      <c r="A71" s="10"/>
+      <c r="B71" s="13"/>
+      <c r="C71" s="40"/>
+      <c r="D71" s="13"/>
       <c r="E71" s="16"/>
       <c r="F71" s="19"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="7"/>
-      <c r="B72" s="10"/>
-      <c r="C72" s="13"/>
-      <c r="D72" s="10"/>
+      <c r="A72" s="10"/>
+      <c r="B72" s="13"/>
+      <c r="C72" s="40"/>
+      <c r="D72" s="13"/>
       <c r="E72" s="16"/>
       <c r="F72" s="19"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="8"/>
-      <c r="B73" s="11"/>
-      <c r="C73" s="14"/>
-      <c r="D73" s="11"/>
+      <c r="A73" s="11"/>
+      <c r="B73" s="14"/>
+      <c r="C73" s="37"/>
+      <c r="D73" s="14"/>
       <c r="E73" s="17"/>
       <c r="F73" s="20"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="B74" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="C74" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="D74" s="9" t="s">
+      <c r="A74" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B74" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="C74" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="D74" s="12" t="s">
         <v>9</v>
       </c>
       <c r="E74" s="15" t="s">
         <v>13</v>
       </c>
       <c r="F74" s="18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="7"/>
-      <c r="B75" s="10"/>
-      <c r="C75" s="13"/>
-      <c r="D75" s="10"/>
+      <c r="A75" s="10"/>
+      <c r="B75" s="13"/>
+      <c r="C75" s="40"/>
+      <c r="D75" s="13"/>
       <c r="E75" s="16"/>
       <c r="F75" s="19"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="7"/>
-      <c r="B76" s="10"/>
-      <c r="C76" s="13"/>
-      <c r="D76" s="10"/>
+      <c r="A76" s="10"/>
+      <c r="B76" s="13"/>
+      <c r="C76" s="40"/>
+      <c r="D76" s="13"/>
       <c r="E76" s="16"/>
       <c r="F76" s="19"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="8"/>
-      <c r="B77" s="11"/>
-      <c r="C77" s="14"/>
-      <c r="D77" s="11"/>
+      <c r="A77" s="11"/>
+      <c r="B77" s="14"/>
+      <c r="C77" s="37"/>
+      <c r="D77" s="14"/>
       <c r="E77" s="17"/>
       <c r="F77" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="121">
+  <mergeCells count="125">
+    <mergeCell ref="I2:I5"/>
+    <mergeCell ref="I14:I17"/>
+    <mergeCell ref="I18:I21"/>
+    <mergeCell ref="I22:I25"/>
+    <mergeCell ref="A74:A77"/>
+    <mergeCell ref="B74:B77"/>
+    <mergeCell ref="C74:C77"/>
+    <mergeCell ref="D74:D77"/>
+    <mergeCell ref="E74:E77"/>
+    <mergeCell ref="F74:F77"/>
+    <mergeCell ref="H14:H17"/>
+    <mergeCell ref="H18:H21"/>
+    <mergeCell ref="F70:F73"/>
+    <mergeCell ref="A70:A73"/>
+    <mergeCell ref="B70:B73"/>
+    <mergeCell ref="C70:C73"/>
+    <mergeCell ref="D70:D73"/>
+    <mergeCell ref="E70:E73"/>
+    <mergeCell ref="F62:F65"/>
+    <mergeCell ref="A66:A69"/>
+    <mergeCell ref="B66:B69"/>
+    <mergeCell ref="C66:C69"/>
+    <mergeCell ref="D66:D69"/>
+    <mergeCell ref="E66:E69"/>
+    <mergeCell ref="F66:F69"/>
+    <mergeCell ref="A62:A65"/>
+    <mergeCell ref="B62:B65"/>
+    <mergeCell ref="C62:C65"/>
+    <mergeCell ref="D62:D65"/>
+    <mergeCell ref="E62:E65"/>
+    <mergeCell ref="F58:F61"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="H2:H5"/>
+    <mergeCell ref="H6:H9"/>
+    <mergeCell ref="A58:A61"/>
+    <mergeCell ref="B58:B61"/>
+    <mergeCell ref="C58:C61"/>
+    <mergeCell ref="D58:D61"/>
+    <mergeCell ref="E58:E61"/>
+    <mergeCell ref="F50:F53"/>
+    <mergeCell ref="A54:A57"/>
+    <mergeCell ref="B54:B57"/>
+    <mergeCell ref="C54:C57"/>
+    <mergeCell ref="D54:D57"/>
+    <mergeCell ref="E54:E57"/>
+    <mergeCell ref="F54:F57"/>
+    <mergeCell ref="A50:A53"/>
+    <mergeCell ref="B50:B53"/>
+    <mergeCell ref="C50:C53"/>
+    <mergeCell ref="D50:D53"/>
+    <mergeCell ref="E50:E53"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="D2:D5"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="F2:F5"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="F10:F13"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="F6:F9"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="E6:E9"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="F18:F21"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="C26:C29"/>
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="E18:E21"/>
+    <mergeCell ref="E14:E17"/>
+    <mergeCell ref="F14:F17"/>
+    <mergeCell ref="D14:D17"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="F22:F25"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="F34:F37"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="F30:F33"/>
+    <mergeCell ref="E34:E37"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="F26:F29"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="E22:E25"/>
+    <mergeCell ref="E26:E29"/>
+    <mergeCell ref="E38:E41"/>
+    <mergeCell ref="D38:D41"/>
     <mergeCell ref="H22:H25"/>
     <mergeCell ref="F42:F45"/>
     <mergeCell ref="C42:C45"/>
@@ -2473,103 +2614,6 @@
     <mergeCell ref="C34:C37"/>
     <mergeCell ref="F38:F41"/>
     <mergeCell ref="D22:D25"/>
-    <mergeCell ref="F22:F25"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="F34:F37"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="F30:F33"/>
-    <mergeCell ref="E34:E37"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="F26:F29"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="E22:E25"/>
-    <mergeCell ref="E26:E29"/>
-    <mergeCell ref="E38:E41"/>
-    <mergeCell ref="D38:D41"/>
-    <mergeCell ref="F18:F21"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="C26:C29"/>
-    <mergeCell ref="D18:D21"/>
-    <mergeCell ref="E18:E21"/>
-    <mergeCell ref="E14:E17"/>
-    <mergeCell ref="F14:F17"/>
-    <mergeCell ref="D14:D17"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="E50:E53"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="D2:D5"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="F2:F5"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="F10:F13"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="D6:D9"/>
-    <mergeCell ref="F6:F9"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="E2:E5"/>
-    <mergeCell ref="E6:E9"/>
-    <mergeCell ref="E10:E13"/>
-    <mergeCell ref="D62:D65"/>
-    <mergeCell ref="E62:E65"/>
-    <mergeCell ref="F58:F61"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="H2:H5"/>
-    <mergeCell ref="H6:H9"/>
-    <mergeCell ref="A58:A61"/>
-    <mergeCell ref="B58:B61"/>
-    <mergeCell ref="C58:C61"/>
-    <mergeCell ref="D58:D61"/>
-    <mergeCell ref="E58:E61"/>
-    <mergeCell ref="F50:F53"/>
-    <mergeCell ref="A54:A57"/>
-    <mergeCell ref="B54:B57"/>
-    <mergeCell ref="C54:C57"/>
-    <mergeCell ref="D54:D57"/>
-    <mergeCell ref="E54:E57"/>
-    <mergeCell ref="F54:F57"/>
-    <mergeCell ref="A50:A53"/>
-    <mergeCell ref="B50:B53"/>
-    <mergeCell ref="C50:C53"/>
-    <mergeCell ref="D50:D53"/>
-    <mergeCell ref="A74:A77"/>
-    <mergeCell ref="B74:B77"/>
-    <mergeCell ref="C74:C77"/>
-    <mergeCell ref="D74:D77"/>
-    <mergeCell ref="E74:E77"/>
-    <mergeCell ref="F74:F77"/>
-    <mergeCell ref="H14:H17"/>
-    <mergeCell ref="H18:H21"/>
-    <mergeCell ref="F70:F73"/>
-    <mergeCell ref="A70:A73"/>
-    <mergeCell ref="B70:B73"/>
-    <mergeCell ref="C70:C73"/>
-    <mergeCell ref="D70:D73"/>
-    <mergeCell ref="E70:E73"/>
-    <mergeCell ref="F62:F65"/>
-    <mergeCell ref="A66:A69"/>
-    <mergeCell ref="B66:B69"/>
-    <mergeCell ref="C66:C69"/>
-    <mergeCell ref="D66:D69"/>
-    <mergeCell ref="E66:E69"/>
-    <mergeCell ref="F66:F69"/>
-    <mergeCell ref="A62:A65"/>
-    <mergeCell ref="B62:B65"/>
-    <mergeCell ref="C62:C65"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>